<commit_message>
first pass at web-ifying the mod
</commit_message>
<xml_diff>
--- a/economics.xlsx
+++ b/economics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\personal\games\workersandresources\workers-and-resources-insane-mode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F3167C-7495-43F5-AE63-6AF9C4CF1952}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324A6A3F-C169-4AF7-977F-FEC5B3E4CBE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{B5883943-4FA7-4C31-ABD9-F72C92AB45FA}"/>
   </bookViews>
@@ -4779,27 +4779,27 @@
         <v>Woodcutting post</v>
       </c>
       <c r="K5" s="4">
-        <f>VLOOKUP($J5,$J$40:$Q$175,2,FALSE)</f>
+        <f t="shared" ref="K5:K30" si="0">VLOOKUP($J5,$J$40:$Q$175,2,FALSE)</f>
         <v>1134</v>
       </c>
       <c r="L5" s="4">
-        <f>VLOOKUP($J5,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" ref="L5:L31" si="1">VLOOKUP($J5,$J$40:$Q$175,3,FALSE)</f>
         <v>37.799999999999997</v>
       </c>
       <c r="M5" s="4">
-        <f>VLOOKUP($J5,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" ref="M5:M31" si="2">VLOOKUP($J5,$J$40:$Q$175,4,FALSE)</f>
         <v>37.799999999999997</v>
       </c>
       <c r="N5" s="3">
-        <f>VLOOKUP($J5,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" ref="N5:N31" si="3">VLOOKUP($J5,$J$40:$Q$175,5,FALSE)</f>
         <v>1</v>
       </c>
       <c r="P5" s="4">
-        <f>VLOOKUP($J5,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" ref="P5:P32" si="4">VLOOKUP($J5,$J$40:$Q$175,7,FALSE)</f>
         <v>4157</v>
       </c>
       <c r="Q5" s="7">
-        <f>VLOOKUP($J5,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" ref="Q5:Q31" si="5">VLOOKUP($J5,$J$40:$Q$175,8,FALSE)</f>
         <v>109.97354497354497</v>
       </c>
       <c r="X5" s="4"/>
@@ -4823,31 +4823,31 @@
       </c>
       <c r="H6" s="5"/>
       <c r="J6" t="str">
-        <f t="shared" ref="J6:J32" si="0">A6</f>
+        <f t="shared" ref="J6:J32" si="6">A6</f>
         <v>Sawmill</v>
       </c>
       <c r="K6" s="4">
-        <f>VLOOKUP($J6,$J$40:$Q$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1059.4000000000005</v>
       </c>
       <c r="L6" s="4">
-        <f>VLOOKUP($J6,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>207.41000000000003</v>
       </c>
       <c r="M6" s="4">
-        <f>VLOOKUP($J6,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>52.970000000000027</v>
       </c>
       <c r="N6" s="3">
-        <f>VLOOKUP($J6,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.25538787908008304</v>
       </c>
       <c r="P6" s="4">
-        <f>VLOOKUP($J6,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q6" s="7">
-        <f>VLOOKUP($J6,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>78.478383990938227</v>
       </c>
       <c r="X6" s="4"/>
@@ -4868,31 +4868,31 @@
       </c>
       <c r="H7" s="5"/>
       <c r="J7" t="str">
+        <f t="shared" si="6"/>
+        <v>Farm</v>
+      </c>
+      <c r="K7" s="4">
         <f t="shared" si="0"/>
-        <v>Farm</v>
-      </c>
-      <c r="K7" s="4">
-        <f>VLOOKUP($J7,$J$40:$Q$175,2,FALSE)</f>
         <v>28.125</v>
       </c>
       <c r="L7" s="4">
-        <f>VLOOKUP($J7,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>28.125</v>
       </c>
       <c r="M7" s="4">
-        <f>VLOOKUP($J7,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>28.125</v>
       </c>
       <c r="N7" s="3">
-        <f>VLOOKUP($J7,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="P7" s="4">
-        <f>VLOOKUP($J7,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q7" s="7">
-        <f>VLOOKUP($J7,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>147.80444444444444</v>
       </c>
       <c r="X7" s="4"/>
@@ -4915,31 +4915,31 @@
       </c>
       <c r="H8" s="5"/>
       <c r="J8" t="str">
+        <f t="shared" si="6"/>
+        <v>Iron Mine</v>
+      </c>
+      <c r="K8" s="4">
         <f t="shared" si="0"/>
-        <v>Iron Mine</v>
-      </c>
-      <c r="K8" s="4">
-        <f>VLOOKUP($J8,$J$40:$Q$175,2,FALSE)</f>
         <v>5000</v>
       </c>
       <c r="L8" s="4">
-        <f>VLOOKUP($J8,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="M8" s="4">
-        <f>VLOOKUP($J8,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="N8" s="3">
-        <f>VLOOKUP($J8,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="P8" s="4">
-        <f>VLOOKUP($J8,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q8" s="7">
-        <f>VLOOKUP($J8,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>207.85</v>
       </c>
       <c r="X8" s="4"/>
@@ -4963,31 +4963,31 @@
       </c>
       <c r="H9" s="5"/>
       <c r="J9" t="str">
+        <f t="shared" si="6"/>
+        <v>Iron Processing</v>
+      </c>
+      <c r="K9" s="4">
         <f t="shared" si="0"/>
-        <v>Iron Processing</v>
-      </c>
-      <c r="K9" s="4">
-        <f>VLOOKUP($J9,$J$40:$Q$175,2,FALSE)</f>
         <v>-209.40000000000009</v>
       </c>
       <c r="L9" s="4">
-        <f>VLOOKUP($J9,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>226.94000000000003</v>
       </c>
       <c r="M9" s="4">
-        <f>VLOOKUP($J9,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-13.960000000000006</v>
       </c>
       <c r="N9" s="3">
-        <f>VLOOKUP($J9,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-6.1514056578831432E-2</v>
       </c>
       <c r="P9" s="4">
-        <f>VLOOKUP($J9,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q9" s="7">
-        <f>VLOOKUP($J9,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-297.77936962750704</v>
       </c>
       <c r="X9" s="4"/>
@@ -5015,31 +5015,31 @@
       </c>
       <c r="H10" s="5"/>
       <c r="J10" t="str">
+        <f t="shared" si="6"/>
+        <v>Steel Mill</v>
+      </c>
+      <c r="K10" s="4">
         <f t="shared" si="0"/>
-        <v>Steel Mill</v>
-      </c>
-      <c r="K10" s="4">
-        <f>VLOOKUP($J10,$J$40:$Q$175,2,FALSE)</f>
         <v>-7311.3499999999985</v>
       </c>
       <c r="L10" s="4">
-        <f>VLOOKUP($J10,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>91.583199999999991</v>
       </c>
       <c r="M10" s="4">
-        <f>VLOOKUP($J10,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-14.622699999999996</v>
       </c>
       <c r="N10" s="3">
-        <f>VLOOKUP($J10,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-0.15966574655613691</v>
       </c>
       <c r="P10" s="4">
-        <f>VLOOKUP($J10,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q10" s="7">
-        <f>VLOOKUP($J10,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-284.28402415422602</v>
       </c>
       <c r="X10" s="4"/>
@@ -5064,31 +5064,31 @@
       </c>
       <c r="H11" s="5"/>
       <c r="J11" t="str">
+        <f t="shared" si="6"/>
+        <v>Coal Mine</v>
+      </c>
+      <c r="K11" s="4">
         <f t="shared" si="0"/>
-        <v>Coal Mine</v>
-      </c>
-      <c r="K11" s="4">
-        <f>VLOOKUP($J11,$J$40:$Q$175,2,FALSE)</f>
         <v>9350.8799999999992</v>
       </c>
       <c r="L11" s="4">
-        <f>VLOOKUP($J11,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>42.503999999999998</v>
       </c>
       <c r="M11" s="4">
-        <f>VLOOKUP($J11,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>42.503999999999998</v>
       </c>
       <c r="N11" s="3">
-        <f>VLOOKUP($J11,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="P11" s="4">
-        <f>VLOOKUP($J11,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q11" s="7">
-        <f>VLOOKUP($J11,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>97.802559759081504</v>
       </c>
     </row>
@@ -5110,31 +5110,31 @@
       </c>
       <c r="H12" s="5"/>
       <c r="J12" t="str">
+        <f t="shared" si="6"/>
+        <v>Coal Processing</v>
+      </c>
+      <c r="K12" s="4">
         <f t="shared" si="0"/>
-        <v>Coal Processing</v>
-      </c>
-      <c r="K12" s="4">
-        <f>VLOOKUP($J12,$J$40:$Q$175,2,FALSE)</f>
         <v>6971.7000000000007</v>
       </c>
       <c r="L12" s="4">
-        <f>VLOOKUP($J12,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>768.72</v>
       </c>
       <c r="M12" s="4">
-        <f>VLOOKUP($J12,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>464.78000000000003</v>
       </c>
       <c r="N12" s="3">
-        <f>VLOOKUP($J12,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.60461546466853988</v>
       </c>
       <c r="P12" s="4">
-        <f>VLOOKUP($J12,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q12" s="7">
-        <f>VLOOKUP($J12,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>8.9440165239468126</v>
       </c>
     </row>
@@ -5156,31 +5156,31 @@
       </c>
       <c r="H13" s="5"/>
       <c r="J13" t="str">
+        <f t="shared" si="6"/>
+        <v>Brick Factory</v>
+      </c>
+      <c r="K13" s="4">
         <f t="shared" si="0"/>
-        <v>Brick Factory</v>
-      </c>
-      <c r="K13" s="4">
-        <f>VLOOKUP($J13,$J$40:$Q$175,2,FALSE)</f>
         <v>-316.26000000000022</v>
       </c>
       <c r="L13" s="4">
-        <f>VLOOKUP($J13,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>47.144399999999997</v>
       </c>
       <c r="M13" s="4">
-        <f>VLOOKUP($J13,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-4.2168000000000028</v>
       </c>
       <c r="N13" s="3">
-        <f>VLOOKUP($J13,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-8.9444345457785082E-2</v>
       </c>
       <c r="P13" s="4">
-        <f>VLOOKUP($J13,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q13" s="7">
-        <f>VLOOKUP($J13,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-985.81863024094037</v>
       </c>
     </row>
@@ -5202,31 +5202,31 @@
       </c>
       <c r="H14" s="5"/>
       <c r="J14" t="str">
+        <f t="shared" si="6"/>
+        <v>Coal Power</v>
+      </c>
+      <c r="K14" s="4">
         <f t="shared" si="0"/>
-        <v>Coal Power</v>
-      </c>
-      <c r="K14" s="4">
-        <f>VLOOKUP($J14,$J$40:$Q$175,2,FALSE)</f>
         <v>3792.48</v>
       </c>
       <c r="L14" s="4">
-        <f>VLOOKUP($J14,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>329.7</v>
       </c>
       <c r="M14" s="4">
-        <f>VLOOKUP($J14,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>189.624</v>
       </c>
       <c r="N14" s="3">
-        <f>VLOOKUP($J14,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.57514103730664246</v>
       </c>
       <c r="P14" s="4">
-        <f>VLOOKUP($J14,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q14" s="7">
-        <f>VLOOKUP($J14,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>21.922330506686919</v>
       </c>
     </row>
@@ -5249,31 +5249,31 @@
       </c>
       <c r="H15" s="5"/>
       <c r="J15" t="str">
+        <f t="shared" si="6"/>
+        <v>Quarry</v>
+      </c>
+      <c r="K15" s="4">
         <f t="shared" si="0"/>
-        <v>Quarry</v>
-      </c>
-      <c r="K15" s="4">
-        <f>VLOOKUP($J15,$J$40:$Q$175,2,FALSE)</f>
         <v>63.000000000000028</v>
       </c>
       <c r="L15" s="4">
-        <f>VLOOKUP($J15,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1.5750000000000006</v>
       </c>
       <c r="M15" s="4">
-        <f>VLOOKUP($J15,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1.5750000000000006</v>
       </c>
       <c r="N15" s="3">
-        <f>VLOOKUP($J15,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="P15" s="4">
-        <f>VLOOKUP($J15,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q15" s="7">
-        <f>VLOOKUP($J15,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>2639.3650793650786</v>
       </c>
     </row>
@@ -5297,31 +5297,31 @@
       </c>
       <c r="H16" s="5"/>
       <c r="J16" t="str">
+        <f t="shared" si="6"/>
+        <v>Gravel Plant</v>
+      </c>
+      <c r="K16" s="4">
         <f t="shared" si="0"/>
-        <v>Gravel Plant</v>
-      </c>
-      <c r="K16" s="4">
-        <f>VLOOKUP($J16,$J$40:$Q$175,2,FALSE)</f>
         <v>-921.57999999999981</v>
       </c>
       <c r="L16" s="4">
-        <f>VLOOKUP($J16,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>35.041333333333334</v>
       </c>
       <c r="M16" s="4">
-        <f>VLOOKUP($J16,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-61.438666666666656</v>
       </c>
       <c r="N16" s="3">
-        <f>VLOOKUP($J16,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-1.7533198888931163</v>
       </c>
       <c r="P16" s="4">
-        <f>VLOOKUP($J16,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q16" s="7">
-        <f>VLOOKUP($J16,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-67.660973545432853</v>
       </c>
     </row>
@@ -5347,31 +5347,31 @@
       </c>
       <c r="H17" s="5"/>
       <c r="J17" t="str">
+        <f t="shared" si="6"/>
+        <v>Cement Plant</v>
+      </c>
+      <c r="K17" s="4">
         <f t="shared" si="0"/>
-        <v>Cement Plant</v>
-      </c>
-      <c r="K17" s="4">
-        <f>VLOOKUP($J17,$J$40:$Q$175,2,FALSE)</f>
         <v>-687.29999999999927</v>
       </c>
       <c r="L17" s="4">
-        <f>VLOOKUP($J17,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>187.00200000000001</v>
       </c>
       <c r="M17" s="4">
-        <f>VLOOKUP($J17,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-22.909999999999975</v>
       </c>
       <c r="N17" s="3">
-        <f>VLOOKUP($J17,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-0.12251205869455928</v>
       </c>
       <c r="P17" s="4">
-        <f>VLOOKUP($J17,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q17" s="7">
-        <f>VLOOKUP($J17,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-181.44914884330007</v>
       </c>
     </row>
@@ -5397,31 +5397,31 @@
       </c>
       <c r="H18" s="5"/>
       <c r="J18" t="str">
+        <f t="shared" si="6"/>
+        <v>Concrete Plant</v>
+      </c>
+      <c r="K18" s="4">
         <f t="shared" si="0"/>
-        <v>Concrete Plant</v>
-      </c>
-      <c r="K18" s="4">
-        <f>VLOOKUP($J18,$J$40:$Q$175,2,FALSE)</f>
         <v>-3055.3999999999996</v>
       </c>
       <c r="L18" s="4">
-        <f>VLOOKUP($J18,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>399.35</v>
       </c>
       <c r="M18" s="4">
-        <f>VLOOKUP($J18,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-611.07999999999993</v>
       </c>
       <c r="N18" s="3">
-        <f>VLOOKUP($J18,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-1.5301865531488668</v>
       </c>
       <c r="P18" s="4">
-        <f>VLOOKUP($J18,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q18" s="7">
-        <f>VLOOKUP($J18,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-6.8027099561432225</v>
       </c>
     </row>
@@ -5443,31 +5443,31 @@
       </c>
       <c r="H19" s="5"/>
       <c r="J19" t="str">
+        <f t="shared" si="6"/>
+        <v>Oil rig</v>
+      </c>
+      <c r="K19" s="4">
         <f t="shared" si="0"/>
-        <v>Oil rig</v>
-      </c>
-      <c r="K19" s="4">
-        <f>VLOOKUP($J19,$J$40:$Q$175,2,FALSE)</f>
         <v>329.86</v>
       </c>
       <c r="L19" s="4">
-        <f>VLOOKUP($J19,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>350.14000000000004</v>
       </c>
       <c r="M19" s="4">
-        <f>VLOOKUP($J19,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>329.86</v>
       </c>
       <c r="N19" s="3">
-        <f>VLOOKUP($J19,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.94208031073284959</v>
       </c>
       <c r="P19" s="4">
-        <f>VLOOKUP($J19,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q19" s="7">
-        <f>VLOOKUP($J19,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>12.602316134117505</v>
       </c>
     </row>
@@ -5493,31 +5493,31 @@
         <v>75</v>
       </c>
       <c r="J20" t="str">
+        <f t="shared" si="6"/>
+        <v>Refinery</v>
+      </c>
+      <c r="K20" s="4">
         <f t="shared" si="0"/>
-        <v>Refinery</v>
-      </c>
-      <c r="K20" s="4">
-        <f>VLOOKUP($J20,$J$40:$Q$175,2,FALSE)</f>
         <v>21259.1</v>
       </c>
       <c r="L20" s="4">
-        <f>VLOOKUP($J20,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>75.548000000000002</v>
       </c>
       <c r="M20" s="4">
-        <f>VLOOKUP($J20,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>42.5182</v>
       </c>
       <c r="N20" s="3">
-        <f>VLOOKUP($J20,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.56279716206914809</v>
       </c>
       <c r="P20" s="4">
-        <f>VLOOKUP($J20,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q20" s="7">
-        <f>VLOOKUP($J20,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>97.769896185633442</v>
       </c>
     </row>
@@ -5543,31 +5543,31 @@
       </c>
       <c r="H21" s="5"/>
       <c r="J21" t="str">
+        <f t="shared" si="6"/>
+        <v>Asphalt</v>
+      </c>
+      <c r="K21" s="4">
         <f t="shared" si="0"/>
-        <v>Asphalt</v>
-      </c>
-      <c r="K21" s="4">
-        <f>VLOOKUP($J21,$J$40:$Q$175,2,FALSE)</f>
         <v>-2581.1500000000005</v>
       </c>
       <c r="L21" s="4">
-        <f>VLOOKUP($J21,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>990.06000000000006</v>
       </c>
       <c r="M21" s="4">
-        <f>VLOOKUP($J21,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-516.23000000000013</v>
       </c>
       <c r="N21" s="3">
-        <f>VLOOKUP($J21,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-0.52141284366604057</v>
       </c>
       <c r="P21" s="4">
-        <f>VLOOKUP($J21,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q21" s="7">
-        <f>VLOOKUP($J21,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-8.0526122077368605</v>
       </c>
     </row>
@@ -5589,31 +5589,31 @@
       </c>
       <c r="H22" s="5"/>
       <c r="J22" t="str">
+        <f t="shared" si="6"/>
+        <v>Livestock Farm</v>
+      </c>
+      <c r="K22" s="4">
         <f t="shared" si="0"/>
-        <v>Livestock Farm</v>
-      </c>
-      <c r="K22" s="4">
-        <f>VLOOKUP($J22,$J$40:$Q$175,2,FALSE)</f>
         <v>7857.5</v>
       </c>
       <c r="L22" s="4">
-        <f>VLOOKUP($J22,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>161.74</v>
       </c>
       <c r="M22" s="4">
-        <f>VLOOKUP($J22,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>157.15</v>
       </c>
       <c r="N22" s="3">
-        <f>VLOOKUP($J22,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.97162112031655745</v>
       </c>
       <c r="P22" s="4">
-        <f>VLOOKUP($J22,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q22" s="7">
-        <f>VLOOKUP($J22,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>26.452433980273625</v>
       </c>
     </row>
@@ -5635,31 +5635,31 @@
       </c>
       <c r="H23" s="5"/>
       <c r="J23" t="str">
+        <f t="shared" si="6"/>
+        <v>Slaughterhouse</v>
+      </c>
+      <c r="K23" s="4">
         <f t="shared" si="0"/>
-        <v>Slaughterhouse</v>
-      </c>
-      <c r="K23" s="4">
-        <f>VLOOKUP($J23,$J$40:$Q$175,2,FALSE)</f>
         <v>-156076.25</v>
       </c>
       <c r="L23" s="4">
-        <f>VLOOKUP($J23,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>5869.3249999999998</v>
       </c>
       <c r="M23" s="4">
-        <f>VLOOKUP($J23,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-3121.5250000000001</v>
       </c>
       <c r="N23" s="3">
-        <f>VLOOKUP($J23,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-0.5318371362976152</v>
       </c>
       <c r="P23" s="4">
-        <f>VLOOKUP($J23,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q23" s="7">
-        <f>VLOOKUP($J23,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-1.3317208736114559</v>
       </c>
     </row>
@@ -5681,31 +5681,31 @@
       </c>
       <c r="H24" s="5"/>
       <c r="J24" t="str">
+        <f t="shared" si="6"/>
+        <v>Food Factory</v>
+      </c>
+      <c r="K24" s="4">
         <f t="shared" si="0"/>
-        <v>Food Factory</v>
-      </c>
-      <c r="K24" s="4">
-        <f>VLOOKUP($J24,$J$40:$Q$175,2,FALSE)</f>
         <v>1300.6999999999998</v>
       </c>
       <c r="L24" s="4">
-        <f>VLOOKUP($J24,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>13.321176470588235</v>
       </c>
       <c r="M24" s="4">
-        <f>VLOOKUP($J24,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>7.6511764705882346</v>
       </c>
       <c r="N24" s="3">
-        <f>VLOOKUP($J24,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.57436191821955307</v>
       </c>
       <c r="P24" s="4">
-        <f>VLOOKUP($J24,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q24" s="7">
-        <f>VLOOKUP($J24,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>543.31513800261405</v>
       </c>
     </row>
@@ -5729,31 +5729,31 @@
       </c>
       <c r="H25" s="5"/>
       <c r="J25" t="str">
+        <f t="shared" si="6"/>
+        <v>Distillery</v>
+      </c>
+      <c r="K25" s="4">
         <f t="shared" si="0"/>
-        <v>Distillery</v>
-      </c>
-      <c r="K25" s="4">
-        <f>VLOOKUP($J25,$J$40:$Q$175,2,FALSE)</f>
         <v>674.83999999999992</v>
       </c>
       <c r="L25" s="4">
-        <f>VLOOKUP($J25,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>14.1534</v>
       </c>
       <c r="M25" s="4">
-        <f>VLOOKUP($J25,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>6.7483999999999993</v>
       </c>
       <c r="N25" s="3">
-        <f>VLOOKUP($J25,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.47680416013113452</v>
       </c>
       <c r="P25" s="4">
-        <f>VLOOKUP($J25,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q25" s="7">
-        <f>VLOOKUP($J25,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>615.99786616086783</v>
       </c>
     </row>
@@ -5779,31 +5779,31 @@
       </c>
       <c r="H26" s="5"/>
       <c r="J26" t="str">
+        <f t="shared" si="6"/>
+        <v>Chemical Plant</v>
+      </c>
+      <c r="K26" s="4">
         <f t="shared" si="0"/>
-        <v>Chemical Plant</v>
-      </c>
-      <c r="K26" s="4">
-        <f>VLOOKUP($J26,$J$40:$Q$175,2,FALSE)</f>
         <v>948.32500000000005</v>
       </c>
       <c r="L26" s="4">
-        <f>VLOOKUP($J26,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>20.630399999999998</v>
       </c>
       <c r="M26" s="4">
-        <f>VLOOKUP($J26,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>18.9665</v>
       </c>
       <c r="N26" s="3">
-        <f>VLOOKUP($J26,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.91934717698154189</v>
       </c>
       <c r="P26" s="4">
-        <f>VLOOKUP($J26,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q26" s="7">
-        <f>VLOOKUP($J26,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>219.17591542983681</v>
       </c>
     </row>
@@ -5829,31 +5829,31 @@
       </c>
       <c r="H27" s="5"/>
       <c r="J27" t="str">
+        <f t="shared" si="6"/>
+        <v>Plastics Factory</v>
+      </c>
+      <c r="K27" s="4">
         <f t="shared" si="0"/>
-        <v>Plastics Factory</v>
-      </c>
-      <c r="K27" s="4">
-        <f>VLOOKUP($J27,$J$40:$Q$175,2,FALSE)</f>
         <v>-12015.849999999997</v>
       </c>
       <c r="L27" s="4">
-        <f>VLOOKUP($J27,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>132.624</v>
       </c>
       <c r="M27" s="4">
-        <f>VLOOKUP($J27,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-120.15849999999996</v>
       </c>
       <c r="N27" s="3">
-        <f>VLOOKUP($J27,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-0.90600871637109404</v>
       </c>
       <c r="P27" s="4">
-        <f>VLOOKUP($J27,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q27" s="7">
-        <f>VLOOKUP($J27,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-34.595971154766417</v>
       </c>
     </row>
@@ -5879,31 +5879,31 @@
       </c>
       <c r="H28" s="5"/>
       <c r="J28" t="str">
+        <f t="shared" si="6"/>
+        <v>Fabric</v>
+      </c>
+      <c r="K28" s="4">
         <f t="shared" si="0"/>
-        <v>Fabric</v>
-      </c>
-      <c r="K28" s="4">
-        <f>VLOOKUP($J28,$J$40:$Q$175,2,FALSE)</f>
         <v>25.085000000000036</v>
       </c>
       <c r="L28" s="4">
-        <f>VLOOKUP($J28,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>16.814499999999999</v>
       </c>
       <c r="M28" s="4">
-        <f>VLOOKUP($J28,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0.25085000000000035</v>
       </c>
       <c r="N28" s="3">
-        <f>VLOOKUP($J28,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1.4918671384816697E-2</v>
       </c>
       <c r="P28" s="4">
-        <f>VLOOKUP($J28,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q28" s="7">
-        <f>VLOOKUP($J28,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>16571.656368347594</v>
       </c>
     </row>
@@ -5925,31 +5925,31 @@
       </c>
       <c r="H29" s="5"/>
       <c r="J29" t="str">
+        <f t="shared" si="6"/>
+        <v>Mech Component</v>
+      </c>
+      <c r="K29" s="4">
         <f t="shared" si="0"/>
-        <v>Mech Component</v>
-      </c>
-      <c r="K29" s="4">
-        <f>VLOOKUP($J29,$J$40:$Q$175,2,FALSE)</f>
         <v>-1108.3899999999994</v>
       </c>
       <c r="L29" s="4">
-        <f>VLOOKUP($J29,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>179.73099999999999</v>
       </c>
       <c r="M29" s="4">
-        <f>VLOOKUP($J29,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-7.3892666666666624</v>
       </c>
       <c r="N29" s="3">
-        <f>VLOOKUP($J29,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-4.1112922460046754E-2</v>
       </c>
       <c r="P29" s="4">
-        <f>VLOOKUP($J29,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q29" s="7">
-        <f>VLOOKUP($J29,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-562.57274064183218</v>
       </c>
     </row>
@@ -5975,31 +5975,31 @@
       </c>
       <c r="H30" s="5"/>
       <c r="J30" t="str">
+        <f t="shared" si="6"/>
+        <v>Elect Comp</v>
+      </c>
+      <c r="K30" s="4">
         <f t="shared" si="0"/>
-        <v>Elect Comp</v>
-      </c>
-      <c r="K30" s="4">
-        <f>VLOOKUP($J30,$J$40:$Q$175,2,FALSE)</f>
         <v>248.00000000000091</v>
       </c>
       <c r="L30" s="4">
-        <f>VLOOKUP($J30,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>42.614973333333332</v>
       </c>
       <c r="M30" s="4">
-        <f>VLOOKUP($J30,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1.6533333333333393</v>
       </c>
       <c r="N30" s="3">
-        <f>VLOOKUP($J30,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>3.8797004996366048E-2</v>
       </c>
       <c r="P30" s="4">
-        <f>VLOOKUP($J30,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q30" s="7">
-        <f>VLOOKUP($J30,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>2514.3145161290231</v>
       </c>
     </row>
@@ -6021,7 +6021,7 @@
       </c>
       <c r="H31" s="5"/>
       <c r="J31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>Clothing Factory</v>
       </c>
       <c r="K31" s="4">
@@ -6029,23 +6029,23 @@
         <v>824.5559999999997</v>
       </c>
       <c r="L31" s="4">
-        <f>VLOOKUP($J31,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>21.773549999999997</v>
       </c>
       <c r="M31" s="4">
-        <f>VLOOKUP($J31,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>10.306949999999997</v>
       </c>
       <c r="N31" s="3">
-        <f>VLOOKUP($J31,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.47337021294184906</v>
       </c>
       <c r="P31" s="4">
-        <f>VLOOKUP($J31,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q31" s="7">
-        <f>VLOOKUP($J31,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>403.32008984229105</v>
       </c>
     </row>
@@ -6071,7 +6071,7 @@
       </c>
       <c r="H32" s="7"/>
       <c r="J32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>Elect Assembly</v>
       </c>
       <c r="K32" s="4">
@@ -6091,7 +6091,7 @@
         <v>4.1474237944260577E-2</v>
       </c>
       <c r="P32" s="4">
-        <f>VLOOKUP($J32,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q32" s="7">
@@ -6297,11 +6297,11 @@
         <v>17</v>
       </c>
       <c r="T38" s="4">
-        <f t="shared" ref="T38:T65" si="1">X38-$T$33</f>
+        <f t="shared" ref="T38:T65" si="7">X38-$T$33</f>
         <v>0.45000000000000018</v>
       </c>
       <c r="U38" s="4">
-        <f t="shared" ref="U38:U65" si="2">Y38+$T$33</f>
+        <f t="shared" ref="U38:U65" si="8">Y38+$T$33</f>
         <v>11.02</v>
       </c>
       <c r="W38" t="s">
@@ -6342,11 +6342,11 @@
         <v>18</v>
       </c>
       <c r="T39" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>11.25</v>
       </c>
       <c r="U39" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>22.95</v>
       </c>
       <c r="W39" t="s">
@@ -6417,11 +6417,11 @@
         <v>19</v>
       </c>
       <c r="T40" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1144.79</v>
       </c>
       <c r="U40" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1275.82</v>
       </c>
       <c r="W40" t="s">
@@ -6439,11 +6439,11 @@
         <v>20</v>
       </c>
       <c r="T41" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>23.96</v>
       </c>
       <c r="U41" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>37.01</v>
       </c>
       <c r="W41" t="s">
@@ -6488,11 +6488,11 @@
         <v>21</v>
       </c>
       <c r="T42" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>69.33</v>
       </c>
       <c r="U42" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>87.16</v>
       </c>
       <c r="W42" t="s">
@@ -6519,11 +6519,11 @@
         <v>22</v>
       </c>
       <c r="T43" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="U43" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>17.16</v>
       </c>
       <c r="W43" t="s">
@@ -6564,11 +6564,11 @@
         <v>23</v>
       </c>
       <c r="T44" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>50.02</v>
       </c>
       <c r="U44" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>65.81</v>
       </c>
       <c r="W44" t="s">
@@ -6639,11 +6639,11 @@
         <v>24</v>
       </c>
       <c r="T45" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>2063.04</v>
       </c>
       <c r="U45" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2290.73</v>
       </c>
       <c r="W45" t="s">
@@ -6661,11 +6661,11 @@
         <v>25</v>
       </c>
       <c r="T46" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>96.09</v>
       </c>
       <c r="U46" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>116.73</v>
       </c>
       <c r="W46" t="s">
@@ -6710,11 +6710,11 @@
         <v>26</v>
       </c>
       <c r="T47" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>10.119999999999999</v>
       </c>
       <c r="U47" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>21.71</v>
       </c>
       <c r="W47" t="s">
@@ -6738,11 +6738,11 @@
         <v>27</v>
       </c>
       <c r="T48" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>32.42</v>
       </c>
       <c r="U48" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>46.36</v>
       </c>
       <c r="W48" t="s">
@@ -6812,11 +6812,11 @@
         <v>28</v>
       </c>
       <c r="T49" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="U49" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>16.060000000000002</v>
       </c>
       <c r="W49" t="s">
@@ -6858,11 +6858,11 @@
         <v>29</v>
       </c>
       <c r="T50" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>228.07</v>
       </c>
       <c r="U50" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>262.61</v>
       </c>
       <c r="W50" t="s">
@@ -6880,11 +6880,11 @@
         <v>30</v>
       </c>
       <c r="T51" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>29.630000000000003</v>
       </c>
       <c r="U51" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>43.28</v>
       </c>
       <c r="W51" t="s">
@@ -6929,11 +6929,11 @@
         <v>31</v>
       </c>
       <c r="T52" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>165.35</v>
       </c>
       <c r="U52" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>193.28</v>
       </c>
       <c r="W52" t="s">
@@ -6957,11 +6957,11 @@
         <v>32</v>
       </c>
       <c r="T53" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>336.29</v>
       </c>
       <c r="U53" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>382.22</v>
       </c>
       <c r="W53" t="s">
@@ -7002,11 +7002,11 @@
         <v>33</v>
       </c>
       <c r="T54" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>235.89</v>
       </c>
       <c r="U54" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>271.25</v>
       </c>
       <c r="W54" t="s">
@@ -7077,11 +7077,11 @@
         <v>34</v>
       </c>
       <c r="T55" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>69.260000000000005</v>
       </c>
       <c r="U55" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>87.08</v>
       </c>
       <c r="W55" t="s">
@@ -7099,11 +7099,11 @@
         <v>35</v>
       </c>
       <c r="T56" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>113.23</v>
       </c>
       <c r="U56" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>135.68</v>
       </c>
       <c r="W56" t="s">
@@ -7148,11 +7148,11 @@
         <v>36</v>
       </c>
       <c r="T57" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1451.57</v>
       </c>
       <c r="U57" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1614.89</v>
       </c>
       <c r="W57" t="s">
@@ -7179,11 +7179,11 @@
         <v>37</v>
       </c>
       <c r="T58" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>2347.73</v>
       </c>
       <c r="U58" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2605.38</v>
       </c>
       <c r="W58" t="s">
@@ -7224,11 +7224,11 @@
         <v>38</v>
       </c>
       <c r="T59" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1617.4</v>
       </c>
       <c r="U59" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1798.17</v>
       </c>
       <c r="W59" t="s">
@@ -7299,11 +7299,11 @@
         <v>39</v>
       </c>
       <c r="T60" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>34.14</v>
       </c>
       <c r="U60" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>48.26</v>
       </c>
       <c r="W60" t="s">
@@ -7321,11 +7321,11 @@
         <v>40</v>
       </c>
       <c r="T61" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>11.41</v>
       </c>
       <c r="U61" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>23.14</v>
       </c>
       <c r="W61" t="s">
@@ -7370,11 +7370,11 @@
         <v>41</v>
       </c>
       <c r="T62" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1682.17</v>
       </c>
       <c r="U62" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1869.77</v>
       </c>
       <c r="W62" t="s">
@@ -7407,11 +7407,11 @@
         <v>42</v>
       </c>
       <c r="T63" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1797.31</v>
       </c>
       <c r="U63" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1997.02</v>
       </c>
       <c r="W63" t="s">
@@ -7452,11 +7452,11 @@
         <v>43</v>
       </c>
       <c r="T64" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>884.16</v>
       </c>
       <c r="U64" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>987.76</v>
       </c>
       <c r="W64" t="s">
@@ -7527,11 +7527,11 @@
         <v>44</v>
       </c>
       <c r="T65" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1871.4</v>
       </c>
       <c r="U65" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2078.92</v>
       </c>
       <c r="W65" t="s">
@@ -9201,11 +9201,11 @@
         <v>963.9</v>
       </c>
       <c r="D135" s="6">
-        <f t="shared" ref="D135:E135" si="3">D134*D132</f>
+        <f t="shared" ref="D135:E135" si="9">D134*D132</f>
         <v>0</v>
       </c>
       <c r="E135" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F135" s="1"/>
@@ -10652,27 +10652,27 @@
         <v>Woodcutting post</v>
       </c>
       <c r="K5" s="4">
-        <f>VLOOKUP($J5,$J$40:$Q$175,2,FALSE)</f>
+        <f t="shared" ref="K5:K32" si="0">VLOOKUP($J5,$J$40:$Q$175,2,FALSE)</f>
         <v>1134</v>
       </c>
       <c r="L5" s="4">
-        <f>VLOOKUP($J5,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" ref="L5:L32" si="1">VLOOKUP($J5,$J$40:$Q$175,3,FALSE)</f>
         <v>37.799999999999997</v>
       </c>
       <c r="M5" s="4">
-        <f>VLOOKUP($J5,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" ref="M5:M32" si="2">VLOOKUP($J5,$J$40:$Q$175,4,FALSE)</f>
         <v>37.799999999999997</v>
       </c>
       <c r="N5" s="3">
-        <f>VLOOKUP($J5,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" ref="N5:N32" si="3">VLOOKUP($J5,$J$40:$Q$175,5,FALSE)</f>
         <v>1</v>
       </c>
       <c r="P5" s="4">
-        <f>VLOOKUP($J5,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" ref="P5:P32" si="4">VLOOKUP($J5,$J$40:$Q$175,7,FALSE)</f>
         <v>4157</v>
       </c>
       <c r="Q5" s="7">
-        <f>VLOOKUP($J5,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" ref="Q5:Q32" si="5">VLOOKUP($J5,$J$40:$Q$175,8,FALSE)</f>
         <v>109.97354497354497</v>
       </c>
       <c r="X5" s="4"/>
@@ -10695,31 +10695,31 @@
       </c>
       <c r="H6"/>
       <c r="J6" t="str">
-        <f t="shared" ref="J6:J33" si="0">A6</f>
+        <f t="shared" ref="J6:J33" si="6">A6</f>
         <v>Sawmill</v>
       </c>
       <c r="K6" s="4">
-        <f>VLOOKUP($J6,$J$40:$Q$175,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1059.4000000000005</v>
       </c>
       <c r="L6" s="4">
-        <f>VLOOKUP($J6,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>207.41000000000003</v>
       </c>
       <c r="M6" s="4">
-        <f>VLOOKUP($J6,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>52.970000000000027</v>
       </c>
       <c r="N6" s="3">
-        <f>VLOOKUP($J6,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.25538787908008304</v>
       </c>
       <c r="P6" s="4">
-        <f>VLOOKUP($J6,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>21764</v>
       </c>
       <c r="Q6" s="7">
-        <f>VLOOKUP($J6,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>410.87407966773628</v>
       </c>
       <c r="X6" s="4"/>
@@ -10740,31 +10740,31 @@
       </c>
       <c r="H7"/>
       <c r="J7" t="str">
+        <f t="shared" si="6"/>
+        <v>Farm</v>
+      </c>
+      <c r="K7" s="4">
         <f t="shared" si="0"/>
-        <v>Farm</v>
-      </c>
-      <c r="K7" s="4">
-        <f>VLOOKUP($J7,$J$40:$Q$175,2,FALSE)</f>
         <v>28.125</v>
       </c>
       <c r="L7" s="4">
-        <f>VLOOKUP($J7,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>28.125</v>
       </c>
       <c r="M7" s="4">
-        <f>VLOOKUP($J7,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>28.125</v>
       </c>
       <c r="N7" s="3">
-        <f>VLOOKUP($J7,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="P7" s="4">
-        <f>VLOOKUP($J7,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q7" s="7">
-        <f>VLOOKUP($J7,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>147.80444444444444</v>
       </c>
       <c r="X7" s="4"/>
@@ -10787,31 +10787,31 @@
       </c>
       <c r="H8" s="5"/>
       <c r="J8" t="str">
+        <f t="shared" si="6"/>
+        <v>Iron Mine</v>
+      </c>
+      <c r="K8" s="4">
         <f t="shared" si="0"/>
-        <v>Iron Mine</v>
-      </c>
-      <c r="K8" s="4">
-        <f>VLOOKUP($J8,$J$40:$Q$175,2,FALSE)</f>
         <v>5000</v>
       </c>
       <c r="L8" s="4">
-        <f>VLOOKUP($J8,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="M8" s="4">
-        <f>VLOOKUP($J8,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="N8" s="3">
-        <f>VLOOKUP($J8,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="P8" s="4">
-        <f>VLOOKUP($J8,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>85018</v>
       </c>
       <c r="Q8" s="7">
-        <f>VLOOKUP($J8,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>4250.8999999999996</v>
       </c>
       <c r="X8" s="4"/>
@@ -10835,31 +10835,31 @@
       </c>
       <c r="H9" s="5"/>
       <c r="J9" t="str">
+        <f t="shared" si="6"/>
+        <v>Iron Processing</v>
+      </c>
+      <c r="K9" s="4">
         <f t="shared" si="0"/>
-        <v>Iron Processing</v>
-      </c>
-      <c r="K9" s="4">
-        <f>VLOOKUP($J9,$J$40:$Q$175,2,FALSE)</f>
         <v>-209.40000000000009</v>
       </c>
       <c r="L9" s="4">
-        <f>VLOOKUP($J9,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>226.94000000000003</v>
       </c>
       <c r="M9" s="4">
-        <f>VLOOKUP($J9,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-13.960000000000006</v>
       </c>
       <c r="N9" s="3">
-        <f>VLOOKUP($J9,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-6.1514056578831432E-2</v>
       </c>
       <c r="P9" s="4">
-        <f>VLOOKUP($J9,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>146810</v>
       </c>
       <c r="Q9" s="7">
-        <f>VLOOKUP($J9,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-10516.475644699136</v>
       </c>
       <c r="X9" s="4"/>
@@ -10887,31 +10887,31 @@
       </c>
       <c r="H10" s="5"/>
       <c r="J10" t="str">
+        <f t="shared" si="6"/>
+        <v>Steel Mill</v>
+      </c>
+      <c r="K10" s="4">
         <f t="shared" si="0"/>
-        <v>Steel Mill</v>
-      </c>
-      <c r="K10" s="4">
-        <f>VLOOKUP($J10,$J$40:$Q$175,2,FALSE)</f>
         <v>-7311.3499999999985</v>
       </c>
       <c r="L10" s="4">
-        <f>VLOOKUP($J10,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>91.583199999999991</v>
       </c>
       <c r="M10" s="4">
-        <f>VLOOKUP($J10,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-14.622699999999996</v>
       </c>
       <c r="N10" s="3">
-        <f>VLOOKUP($J10,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-0.15966574655613691</v>
       </c>
       <c r="P10" s="4">
-        <f>VLOOKUP($J10,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>257030</v>
       </c>
       <c r="Q10" s="7">
-        <f>VLOOKUP($J10,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-17577.465174010274</v>
       </c>
       <c r="X10" s="4"/>
@@ -10936,31 +10936,31 @@
       </c>
       <c r="H11" s="5"/>
       <c r="J11" t="str">
+        <f t="shared" si="6"/>
+        <v>Coal Mine</v>
+      </c>
+      <c r="K11" s="4">
         <f t="shared" si="0"/>
-        <v>Coal Mine</v>
-      </c>
-      <c r="K11" s="4">
-        <f>VLOOKUP($J11,$J$40:$Q$175,2,FALSE)</f>
         <v>9350.8799999999992</v>
       </c>
       <c r="L11" s="4">
-        <f>VLOOKUP($J11,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>42.503999999999998</v>
       </c>
       <c r="M11" s="4">
-        <f>VLOOKUP($J11,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>42.503999999999998</v>
       </c>
       <c r="N11" s="3">
-        <f>VLOOKUP($J11,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="P11" s="4">
-        <f>VLOOKUP($J11,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>84568</v>
       </c>
       <c r="Q11" s="7">
-        <f>VLOOKUP($J11,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1989.6480331262942</v>
       </c>
     </row>
@@ -10982,31 +10982,31 @@
       </c>
       <c r="H12" s="5"/>
       <c r="J12" t="str">
+        <f t="shared" si="6"/>
+        <v>Coal Processing</v>
+      </c>
+      <c r="K12" s="4">
         <f t="shared" si="0"/>
-        <v>Coal Processing</v>
-      </c>
-      <c r="K12" s="4">
-        <f>VLOOKUP($J12,$J$40:$Q$175,2,FALSE)</f>
         <v>2647.6499999999996</v>
       </c>
       <c r="L12" s="4">
-        <f>VLOOKUP($J12,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>240.22499999999999</v>
       </c>
       <c r="M12" s="4">
-        <f>VLOOKUP($J12,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>88.254999999999981</v>
       </c>
       <c r="N12" s="3">
-        <f>VLOOKUP($J12,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.36738474346966382</v>
       </c>
       <c r="P12" s="4">
-        <f>VLOOKUP($J12,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>146810</v>
       </c>
       <c r="Q12" s="7">
-        <f>VLOOKUP($J12,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1663.4751572148889</v>
       </c>
     </row>
@@ -11028,31 +11028,31 @@
       </c>
       <c r="H13" s="5"/>
       <c r="J13" t="str">
+        <f t="shared" si="6"/>
+        <v>Brick Factory</v>
+      </c>
+      <c r="K13" s="4">
         <f t="shared" si="0"/>
-        <v>Brick Factory</v>
-      </c>
-      <c r="K13" s="4">
-        <f>VLOOKUP($J13,$J$40:$Q$175,2,FALSE)</f>
         <v>-316.26000000000022</v>
       </c>
       <c r="L13" s="4">
-        <f>VLOOKUP($J13,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>47.144399999999997</v>
       </c>
       <c r="M13" s="4">
-        <f>VLOOKUP($J13,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-4.2168000000000028</v>
       </c>
       <c r="N13" s="3">
-        <f>VLOOKUP($J13,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-8.9444345457785082E-2</v>
       </c>
       <c r="P13" s="4">
-        <f>VLOOKUP($J13,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>56668</v>
       </c>
       <c r="Q13" s="7">
-        <f>VLOOKUP($J13,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-13438.626446594564</v>
       </c>
     </row>
@@ -11074,31 +11074,31 @@
       </c>
       <c r="H14" s="5"/>
       <c r="J14" t="str">
+        <f t="shared" si="6"/>
+        <v>Coal Power</v>
+      </c>
+      <c r="K14" s="4">
         <f t="shared" si="0"/>
-        <v>Coal Power</v>
-      </c>
-      <c r="K14" s="4">
-        <f>VLOOKUP($J14,$J$40:$Q$175,2,FALSE)</f>
         <v>1908.48</v>
       </c>
       <c r="L14" s="4">
-        <f>VLOOKUP($J14,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>117.75</v>
       </c>
       <c r="M14" s="4">
-        <f>VLOOKUP($J14,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>47.712000000000003</v>
       </c>
       <c r="N14" s="3">
-        <f>VLOOKUP($J14,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.40519745222929937</v>
       </c>
       <c r="P14" s="4">
-        <f>VLOOKUP($J14,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>252962</v>
       </c>
       <c r="Q14" s="7">
-        <f>VLOOKUP($J14,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>5301.8527833668677</v>
       </c>
     </row>
@@ -11121,31 +11121,31 @@
       </c>
       <c r="H15" s="5"/>
       <c r="J15" t="str">
+        <f t="shared" si="6"/>
+        <v>Quarry</v>
+      </c>
+      <c r="K15" s="4">
         <f t="shared" si="0"/>
-        <v>Quarry</v>
-      </c>
-      <c r="K15" s="4">
-        <f>VLOOKUP($J15,$J$40:$Q$175,2,FALSE)</f>
         <v>63.000000000000028</v>
       </c>
       <c r="L15" s="4">
-        <f>VLOOKUP($J15,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1.5750000000000006</v>
       </c>
       <c r="M15" s="4">
-        <f>VLOOKUP($J15,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1.5750000000000006</v>
       </c>
       <c r="N15" s="3">
-        <f>VLOOKUP($J15,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="P15" s="4">
-        <f>VLOOKUP($J15,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>1641</v>
       </c>
       <c r="Q15" s="7">
-        <f>VLOOKUP($J15,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1041.9047619047615</v>
       </c>
     </row>
@@ -11169,31 +11169,31 @@
       </c>
       <c r="H16" s="5"/>
       <c r="J16" t="str">
+        <f t="shared" si="6"/>
+        <v>Gravel Plant</v>
+      </c>
+      <c r="K16" s="4">
         <f t="shared" si="0"/>
-        <v>Gravel Plant</v>
-      </c>
-      <c r="K16" s="4">
-        <f>VLOOKUP($J16,$J$40:$Q$175,2,FALSE)</f>
         <v>-921.57999999999981</v>
       </c>
       <c r="L16" s="4">
-        <f>VLOOKUP($J16,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>35.041333333333334</v>
       </c>
       <c r="M16" s="4">
-        <f>VLOOKUP($J16,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-61.438666666666656</v>
       </c>
       <c r="N16" s="3">
-        <f>VLOOKUP($J16,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-1.7533198888931163</v>
       </c>
       <c r="P16" s="4">
-        <f>VLOOKUP($J16,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>36782</v>
       </c>
       <c r="Q16" s="7">
-        <f>VLOOKUP($J16,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-598.67835673517231</v>
       </c>
     </row>
@@ -11219,31 +11219,31 @@
       </c>
       <c r="H17" s="5"/>
       <c r="J17" t="str">
+        <f t="shared" si="6"/>
+        <v>Cement Plant</v>
+      </c>
+      <c r="K17" s="4">
         <f t="shared" si="0"/>
-        <v>Cement Plant</v>
-      </c>
-      <c r="K17" s="4">
-        <f>VLOOKUP($J17,$J$40:$Q$175,2,FALSE)</f>
         <v>-687.29999999999927</v>
       </c>
       <c r="L17" s="4">
-        <f>VLOOKUP($J17,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>187.00200000000001</v>
       </c>
       <c r="M17" s="4">
-        <f>VLOOKUP($J17,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-22.909999999999975</v>
       </c>
       <c r="N17" s="3">
-        <f>VLOOKUP($J17,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-0.12251205869455928</v>
       </c>
       <c r="P17" s="4">
-        <f>VLOOKUP($J17,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>203603</v>
       </c>
       <c r="Q17" s="7">
-        <f>VLOOKUP($J17,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-8887.0798777826385</v>
       </c>
     </row>
@@ -11269,31 +11269,31 @@
       </c>
       <c r="H18" s="5"/>
       <c r="J18" t="str">
+        <f t="shared" si="6"/>
+        <v>Concrete Plant</v>
+      </c>
+      <c r="K18" s="4">
         <f t="shared" si="0"/>
-        <v>Concrete Plant</v>
-      </c>
-      <c r="K18" s="4">
-        <f>VLOOKUP($J18,$J$40:$Q$175,2,FALSE)</f>
         <v>-3055.3999999999996</v>
       </c>
       <c r="L18" s="4">
-        <f>VLOOKUP($J18,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>399.35</v>
       </c>
       <c r="M18" s="4">
-        <f>VLOOKUP($J18,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-611.07999999999993</v>
       </c>
       <c r="N18" s="3">
-        <f>VLOOKUP($J18,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-1.5301865531488668</v>
       </c>
       <c r="P18" s="4">
-        <f>VLOOKUP($J18,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>34720</v>
       </c>
       <c r="Q18" s="7">
-        <f>VLOOKUP($J18,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-56.817437978660735</v>
       </c>
     </row>
@@ -11315,31 +11315,31 @@
       </c>
       <c r="H19" s="5"/>
       <c r="J19" t="str">
+        <f t="shared" si="6"/>
+        <v>Oil rig</v>
+      </c>
+      <c r="K19" s="4">
         <f t="shared" si="0"/>
-        <v>Oil rig</v>
-      </c>
-      <c r="K19" s="4">
-        <f>VLOOKUP($J19,$J$40:$Q$175,2,FALSE)</f>
         <v>154.79000000000002</v>
       </c>
       <c r="L19" s="4">
-        <f>VLOOKUP($J19,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>175.07000000000002</v>
       </c>
       <c r="M19" s="4">
-        <f>VLOOKUP($J19,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>154.79000000000002</v>
       </c>
       <c r="N19" s="3">
-        <f>VLOOKUP($J19,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.8841606214656994</v>
       </c>
       <c r="P19" s="4">
-        <f>VLOOKUP($J19,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>6069</v>
       </c>
       <c r="Q19" s="7">
-        <f>VLOOKUP($J19,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>39.207959170489048</v>
       </c>
     </row>
@@ -11365,31 +11365,31 @@
         <v>60</v>
       </c>
       <c r="J20" t="str">
+        <f t="shared" si="6"/>
+        <v>Refinery</v>
+      </c>
+      <c r="K20" s="4">
         <f t="shared" si="0"/>
-        <v>Refinery</v>
-      </c>
-      <c r="K20" s="4">
-        <f>VLOOKUP($J20,$J$40:$Q$175,2,FALSE)</f>
         <v>13704.299999999996</v>
       </c>
       <c r="L20" s="4">
-        <f>VLOOKUP($J20,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>60.438399999999994</v>
       </c>
       <c r="M20" s="4">
-        <f>VLOOKUP($J20,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>27.408599999999993</v>
       </c>
       <c r="N20" s="3">
-        <f>VLOOKUP($J20,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.45349645258643501</v>
       </c>
       <c r="P20" s="4">
-        <f>VLOOKUP($J20,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>296868</v>
       </c>
       <c r="Q20" s="7">
-        <f>VLOOKUP($J20,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>10831.198966747668</v>
       </c>
     </row>
@@ -11415,31 +11415,31 @@
       </c>
       <c r="H21" s="5"/>
       <c r="J21" t="str">
+        <f t="shared" si="6"/>
+        <v>Asphalt</v>
+      </c>
+      <c r="K21" s="4">
         <f t="shared" si="0"/>
-        <v>Asphalt</v>
-      </c>
-      <c r="K21" s="4">
-        <f>VLOOKUP($J21,$J$40:$Q$175,2,FALSE)</f>
         <v>-2581.1500000000005</v>
       </c>
       <c r="L21" s="4">
-        <f>VLOOKUP($J21,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>990.06000000000006</v>
       </c>
       <c r="M21" s="4">
-        <f>VLOOKUP($J21,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-516.23000000000013</v>
       </c>
       <c r="N21" s="3">
-        <f>VLOOKUP($J21,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-0.52141284366604057</v>
       </c>
       <c r="P21" s="4">
-        <f>VLOOKUP($J21,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>38940</v>
       </c>
       <c r="Q21" s="7">
-        <f>VLOOKUP($J21,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-75.431493714042176</v>
       </c>
     </row>
@@ -11461,31 +11461,31 @@
       </c>
       <c r="H22" s="5"/>
       <c r="J22" t="str">
+        <f t="shared" si="6"/>
+        <v>Livestock Farm</v>
+      </c>
+      <c r="K22" s="4">
         <f t="shared" si="0"/>
-        <v>Livestock Farm</v>
-      </c>
-      <c r="K22" s="4">
-        <f>VLOOKUP($J22,$J$40:$Q$175,2,FALSE)</f>
         <v>4622.7000000000007</v>
       </c>
       <c r="L22" s="4">
-        <f>VLOOKUP($J22,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>97.044000000000011</v>
       </c>
       <c r="M22" s="4">
-        <f>VLOOKUP($J22,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>92.454000000000008</v>
       </c>
       <c r="N22" s="3">
-        <f>VLOOKUP($J22,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.95270186719426242</v>
       </c>
       <c r="P22" s="4">
-        <f>VLOOKUP($J22,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>47934</v>
       </c>
       <c r="Q22" s="7">
-        <f>VLOOKUP($J22,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>518.46323577130238</v>
       </c>
     </row>
@@ -11507,31 +11507,31 @@
       </c>
       <c r="H23" s="5"/>
       <c r="J23" t="str">
+        <f t="shared" si="6"/>
+        <v>Slaughterhouse</v>
+      </c>
+      <c r="K23" s="4">
         <f t="shared" si="0"/>
-        <v>Slaughterhouse</v>
-      </c>
-      <c r="K23" s="4">
-        <f>VLOOKUP($J23,$J$40:$Q$175,2,FALSE)</f>
         <v>-156076.25</v>
       </c>
       <c r="L23" s="4">
-        <f>VLOOKUP($J23,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>5869.3249999999998</v>
       </c>
       <c r="M23" s="4">
-        <f>VLOOKUP($J23,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-3121.5250000000001</v>
       </c>
       <c r="N23" s="3">
-        <f>VLOOKUP($J23,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-0.5318371362976152</v>
       </c>
       <c r="P23" s="4">
-        <f>VLOOKUP($J23,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>35621</v>
       </c>
       <c r="Q23" s="7">
-        <f>VLOOKUP($J23,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-11.411409487349932</v>
       </c>
     </row>
@@ -11553,31 +11553,31 @@
       </c>
       <c r="H24" s="5"/>
       <c r="J24" t="str">
+        <f t="shared" si="6"/>
+        <v>Food Factory</v>
+      </c>
+      <c r="K24" s="4">
         <f t="shared" si="0"/>
-        <v>Food Factory</v>
-      </c>
-      <c r="K24" s="4">
-        <f>VLOOKUP($J24,$J$40:$Q$175,2,FALSE)</f>
         <v>1300.6999999999998</v>
       </c>
       <c r="L24" s="4">
-        <f>VLOOKUP($J24,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>13.321176470588235</v>
       </c>
       <c r="M24" s="4">
-        <f>VLOOKUP($J24,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>7.6511764705882346</v>
       </c>
       <c r="N24" s="3">
-        <f>VLOOKUP($J24,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.57436191821955307</v>
       </c>
       <c r="P24" s="4">
-        <f>VLOOKUP($J24,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>71504</v>
       </c>
       <c r="Q24" s="7">
-        <f>VLOOKUP($J24,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>9345.4908895210283</v>
       </c>
     </row>
@@ -11601,31 +11601,31 @@
       </c>
       <c r="H25" s="5"/>
       <c r="J25" t="str">
+        <f t="shared" si="6"/>
+        <v>Distillery</v>
+      </c>
+      <c r="K25" s="4">
         <f t="shared" si="0"/>
-        <v>Distillery</v>
-      </c>
-      <c r="K25" s="4">
-        <f>VLOOKUP($J25,$J$40:$Q$175,2,FALSE)</f>
         <v>674.83999999999992</v>
       </c>
       <c r="L25" s="4">
-        <f>VLOOKUP($J25,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>14.1534</v>
       </c>
       <c r="M25" s="4">
-        <f>VLOOKUP($J25,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>6.7483999999999993</v>
       </c>
       <c r="N25" s="3">
-        <f>VLOOKUP($J25,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.47680416013113452</v>
       </c>
       <c r="P25" s="4">
-        <f>VLOOKUP($J25,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>37951</v>
       </c>
       <c r="Q25" s="7">
-        <f>VLOOKUP($J25,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>5623.7033963606191</v>
       </c>
     </row>
@@ -11651,31 +11651,31 @@
       </c>
       <c r="H26" s="5"/>
       <c r="J26" t="str">
+        <f t="shared" si="6"/>
+        <v>Chemical Plant</v>
+      </c>
+      <c r="K26" s="4">
         <f t="shared" si="0"/>
-        <v>Chemical Plant</v>
-      </c>
-      <c r="K26" s="4">
-        <f>VLOOKUP($J26,$J$40:$Q$175,2,FALSE)</f>
         <v>948.32500000000005</v>
       </c>
       <c r="L26" s="4">
-        <f>VLOOKUP($J26,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>20.630399999999998</v>
       </c>
       <c r="M26" s="4">
-        <f>VLOOKUP($J26,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>18.9665</v>
       </c>
       <c r="N26" s="3">
-        <f>VLOOKUP($J26,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.91934717698154189</v>
       </c>
       <c r="P26" s="4">
-        <f>VLOOKUP($J26,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q26" s="7">
-        <f>VLOOKUP($J26,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -11701,31 +11701,31 @@
       </c>
       <c r="H27" s="5"/>
       <c r="J27" t="str">
+        <f t="shared" si="6"/>
+        <v>Plastics Factory</v>
+      </c>
+      <c r="K27" s="4">
         <f t="shared" si="0"/>
-        <v>Plastics Factory</v>
-      </c>
-      <c r="K27" s="4">
-        <f>VLOOKUP($J27,$J$40:$Q$175,2,FALSE)</f>
         <v>-12015.849999999997</v>
       </c>
       <c r="L27" s="4">
-        <f>VLOOKUP($J27,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>132.624</v>
       </c>
       <c r="M27" s="4">
-        <f>VLOOKUP($J27,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-120.15849999999996</v>
       </c>
       <c r="N27" s="3">
-        <f>VLOOKUP($J27,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-0.90600871637109404</v>
       </c>
       <c r="P27" s="4">
-        <f>VLOOKUP($J27,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>33226</v>
       </c>
       <c r="Q27" s="7">
-        <f>VLOOKUP($J27,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-276.51809901088984</v>
       </c>
     </row>
@@ -11751,31 +11751,31 @@
       </c>
       <c r="H28" s="5"/>
       <c r="J28" t="str">
+        <f t="shared" si="6"/>
+        <v>Fabric</v>
+      </c>
+      <c r="K28" s="4">
         <f t="shared" si="0"/>
-        <v>Fabric</v>
-      </c>
-      <c r="K28" s="4">
-        <f>VLOOKUP($J28,$J$40:$Q$175,2,FALSE)</f>
         <v>25.085000000000036</v>
       </c>
       <c r="L28" s="4">
-        <f>VLOOKUP($J28,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>16.814499999999999</v>
       </c>
       <c r="M28" s="4">
-        <f>VLOOKUP($J28,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0.25085000000000035</v>
       </c>
       <c r="N28" s="3">
-        <f>VLOOKUP($J28,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1.4918671384816697E-2</v>
       </c>
       <c r="P28" s="4">
-        <f>VLOOKUP($J28,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>35900</v>
       </c>
       <c r="Q28" s="7">
-        <f>VLOOKUP($J28,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>143113.41439107017</v>
       </c>
     </row>
@@ -11797,31 +11797,31 @@
       </c>
       <c r="H29" s="5"/>
       <c r="J29" t="str">
+        <f t="shared" si="6"/>
+        <v>Mech Component</v>
+      </c>
+      <c r="K29" s="4">
         <f t="shared" si="0"/>
-        <v>Mech Component</v>
-      </c>
-      <c r="K29" s="4">
-        <f>VLOOKUP($J29,$J$40:$Q$175,2,FALSE)</f>
         <v>-1108.3899999999994</v>
       </c>
       <c r="L29" s="4">
-        <f>VLOOKUP($J29,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>179.73099999999999</v>
       </c>
       <c r="M29" s="4">
-        <f>VLOOKUP($J29,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-7.3892666666666624</v>
       </c>
       <c r="N29" s="3">
-        <f>VLOOKUP($J29,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-4.1112922460046754E-2</v>
       </c>
       <c r="P29" s="4">
-        <f>VLOOKUP($J29,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q29" s="7">
-        <f>VLOOKUP($J29,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -11847,31 +11847,31 @@
       </c>
       <c r="H30" s="5"/>
       <c r="J30" t="str">
+        <f t="shared" si="6"/>
+        <v>Elect Comp</v>
+      </c>
+      <c r="K30" s="4">
         <f t="shared" si="0"/>
-        <v>Elect Comp</v>
-      </c>
-      <c r="K30" s="4">
-        <f>VLOOKUP($J30,$J$40:$Q$175,2,FALSE)</f>
         <v>248.00000000000091</v>
       </c>
       <c r="L30" s="4">
-        <f>VLOOKUP($J30,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>42.614973333333332</v>
       </c>
       <c r="M30" s="4">
-        <f>VLOOKUP($J30,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1.6533333333333393</v>
       </c>
       <c r="N30" s="3">
-        <f>VLOOKUP($J30,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>3.8797004996366048E-2</v>
       </c>
       <c r="P30" s="4">
-        <f>VLOOKUP($J30,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q30" s="7">
-        <f>VLOOKUP($J30,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -11893,31 +11893,31 @@
       </c>
       <c r="H31" s="5"/>
       <c r="J31" t="str">
+        <f t="shared" si="6"/>
+        <v>Clothing Factory</v>
+      </c>
+      <c r="K31" s="4">
         <f t="shared" si="0"/>
-        <v>Clothing Factory</v>
-      </c>
-      <c r="K31" s="4">
-        <f>VLOOKUP($J31,$J$40:$Q$175,2,FALSE)</f>
         <v>243.928</v>
       </c>
       <c r="L31" s="4">
-        <f>VLOOKUP($J31,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>14.515700000000001</v>
       </c>
       <c r="M31" s="4">
-        <f>VLOOKUP($J31,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>3.0491000000000001</v>
       </c>
       <c r="N31" s="3">
-        <f>VLOOKUP($J31,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.21005531941277375</v>
       </c>
       <c r="P31" s="4">
-        <f>VLOOKUP($J31,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>49231</v>
       </c>
       <c r="Q31" s="7">
-        <f>VLOOKUP($J31,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>16146.075891246599</v>
       </c>
     </row>
@@ -11943,31 +11943,31 @@
       </c>
       <c r="H32" s="5"/>
       <c r="J32" t="str">
+        <f t="shared" si="6"/>
+        <v>Elect Assembly</v>
+      </c>
+      <c r="K32" s="4">
         <f t="shared" si="0"/>
-        <v>Elect Assembly</v>
-      </c>
-      <c r="K32" s="4">
-        <f>VLOOKUP($J32,$J$40:$Q$175,2,FALSE)</f>
         <v>349.26700000000164</v>
       </c>
       <c r="L32" s="4">
-        <f>VLOOKUP($J32,$J$40:$Q$175,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>56.14200000000001</v>
       </c>
       <c r="M32" s="4">
-        <f>VLOOKUP($J32,$J$40:$Q$175,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>2.3284466666666774</v>
       </c>
       <c r="N32" s="3">
-        <f>VLOOKUP($J32,$J$40:$Q$175,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>4.1474237944260577E-2</v>
       </c>
       <c r="P32" s="4">
-        <f>VLOOKUP($J32,$J$40:$Q$175,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q32" s="7">
-        <f>VLOOKUP($J32,$J$40:$Q$175,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -11992,7 +11992,7 @@
       </c>
       <c r="H33" s="7"/>
       <c r="J33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>Prefab Factory</v>
       </c>
       <c r="K33" s="4">
@@ -12170,11 +12170,11 @@
         <v>17</v>
       </c>
       <c r="T38" s="4">
-        <f t="shared" ref="T38:T65" si="1">X38-$T$33</f>
+        <f t="shared" ref="T38:T65" si="7">X38-$T$33</f>
         <v>0.45000000000000018</v>
       </c>
       <c r="U38" s="4">
-        <f t="shared" ref="U38:U65" si="2">Y38+$T$33</f>
+        <f t="shared" ref="U38:U65" si="8">Y38+$T$33</f>
         <v>11.02</v>
       </c>
       <c r="W38" t="s">
@@ -12216,11 +12216,11 @@
         <v>18</v>
       </c>
       <c r="T39" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>11.25</v>
       </c>
       <c r="U39" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>22.95</v>
       </c>
       <c r="W39" t="s">
@@ -12290,11 +12290,11 @@
         <v>19</v>
       </c>
       <c r="T40" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1144.79</v>
       </c>
       <c r="U40" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1275.82</v>
       </c>
       <c r="W40" t="s">
@@ -12312,11 +12312,11 @@
         <v>20</v>
       </c>
       <c r="T41" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>23.96</v>
       </c>
       <c r="U41" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>37.01</v>
       </c>
       <c r="W41" t="s">
@@ -12361,11 +12361,11 @@
         <v>21</v>
       </c>
       <c r="T42" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>69.33</v>
       </c>
       <c r="U42" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>87.16</v>
       </c>
       <c r="W42" t="s">
@@ -12392,11 +12392,11 @@
         <v>22</v>
       </c>
       <c r="T43" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="U43" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>17.16</v>
       </c>
       <c r="W43" t="s">
@@ -12438,11 +12438,11 @@
         <v>23</v>
       </c>
       <c r="T44" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>50.02</v>
       </c>
       <c r="U44" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>65.81</v>
       </c>
       <c r="W44" t="s">
@@ -12512,11 +12512,11 @@
         <v>24</v>
       </c>
       <c r="T45" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>2063.04</v>
       </c>
       <c r="U45" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2290.73</v>
       </c>
       <c r="W45" t="s">
@@ -12534,11 +12534,11 @@
         <v>25</v>
       </c>
       <c r="T46" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>96.09</v>
       </c>
       <c r="U46" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>116.73</v>
       </c>
       <c r="W46" t="s">
@@ -12583,11 +12583,11 @@
         <v>26</v>
       </c>
       <c r="T47" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>10.119999999999999</v>
       </c>
       <c r="U47" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>21.71</v>
       </c>
       <c r="W47" t="s">
@@ -12611,11 +12611,11 @@
         <v>27</v>
       </c>
       <c r="T48" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>32.42</v>
       </c>
       <c r="U48" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>46.36</v>
       </c>
       <c r="W48" t="s">
@@ -12657,11 +12657,11 @@
         <v>28</v>
       </c>
       <c r="T49" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="U49" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>16.060000000000002</v>
       </c>
       <c r="W49" t="s">
@@ -12731,11 +12731,11 @@
         <v>29</v>
       </c>
       <c r="T50" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>228.07</v>
       </c>
       <c r="U50" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>262.61</v>
       </c>
       <c r="W50" t="s">
@@ -12753,11 +12753,11 @@
         <v>30</v>
       </c>
       <c r="T51" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>29.630000000000003</v>
       </c>
       <c r="U51" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>43.28</v>
       </c>
       <c r="W51" t="s">
@@ -12802,11 +12802,11 @@
         <v>31</v>
       </c>
       <c r="T52" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>165.35</v>
       </c>
       <c r="U52" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>193.28</v>
       </c>
       <c r="W52" t="s">
@@ -12830,11 +12830,11 @@
         <v>32</v>
       </c>
       <c r="T53" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>336.29</v>
       </c>
       <c r="U53" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>382.22</v>
       </c>
       <c r="W53" t="s">
@@ -12876,11 +12876,11 @@
         <v>33</v>
       </c>
       <c r="T54" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>235.89</v>
       </c>
       <c r="U54" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>271.25</v>
       </c>
       <c r="W54" t="s">
@@ -12950,11 +12950,11 @@
         <v>34</v>
       </c>
       <c r="T55" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>69.260000000000005</v>
       </c>
       <c r="U55" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>87.08</v>
       </c>
       <c r="W55" t="s">
@@ -12972,11 +12972,11 @@
         <v>35</v>
       </c>
       <c r="T56" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>113.23</v>
       </c>
       <c r="U56" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>135.68</v>
       </c>
       <c r="W56" t="s">
@@ -13021,11 +13021,11 @@
         <v>36</v>
       </c>
       <c r="T57" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1451.57</v>
       </c>
       <c r="U57" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1614.89</v>
       </c>
       <c r="W57" t="s">
@@ -13052,11 +13052,11 @@
         <v>37</v>
       </c>
       <c r="T58" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>2347.73</v>
       </c>
       <c r="U58" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2605.38</v>
       </c>
       <c r="W58" t="s">
@@ -13098,11 +13098,11 @@
         <v>38</v>
       </c>
       <c r="T59" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1617.4</v>
       </c>
       <c r="U59" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1798.17</v>
       </c>
       <c r="W59" t="s">
@@ -13172,11 +13172,11 @@
         <v>39</v>
       </c>
       <c r="T60" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>34.14</v>
       </c>
       <c r="U60" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>48.26</v>
       </c>
       <c r="W60" t="s">
@@ -13194,11 +13194,11 @@
         <v>40</v>
       </c>
       <c r="T61" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>11.41</v>
       </c>
       <c r="U61" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>23.14</v>
       </c>
       <c r="W61" t="s">
@@ -13243,11 +13243,11 @@
         <v>41</v>
       </c>
       <c r="T62" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1682.17</v>
       </c>
       <c r="U62" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1869.77</v>
       </c>
       <c r="W62" t="s">
@@ -13280,11 +13280,11 @@
         <v>42</v>
       </c>
       <c r="T63" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1797.31</v>
       </c>
       <c r="U63" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1997.02</v>
       </c>
       <c r="W63" t="s">
@@ -13326,11 +13326,11 @@
         <v>43</v>
       </c>
       <c r="T64" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>884.16</v>
       </c>
       <c r="U64" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>987.76</v>
       </c>
       <c r="W64" t="s">
@@ -13400,11 +13400,11 @@
         <v>44</v>
       </c>
       <c r="T65" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1871.4</v>
       </c>
       <c r="U65" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2078.92</v>
       </c>
       <c r="W65" t="s">
@@ -15075,11 +15075,11 @@
         <v>963.9</v>
       </c>
       <c r="D135" s="6">
-        <f t="shared" ref="D135:E135" si="3">D134*D132</f>
+        <f t="shared" ref="D135:E135" si="9">D134*D132</f>
         <v>0</v>
       </c>
       <c r="E135" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F135" s="1"/>
@@ -16441,7 +16441,7 @@
   <dimension ref="A2:Y217"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16557,27 +16557,27 @@
         <v>Woodcutting Post</v>
       </c>
       <c r="K5" s="4">
-        <f>VLOOKUP($J5,$J$44:$Q$179,2,FALSE)</f>
+        <f t="shared" ref="K5:K25" si="0">VLOOKUP($J5,$J$44:$Q$179,2,FALSE)</f>
         <v>1662.55</v>
       </c>
       <c r="L5" s="4">
-        <f>VLOOKUP($J5,$J$44:$Q$179,3,FALSE)</f>
+        <f t="shared" ref="L5:L25" si="1">VLOOKUP($J5,$J$44:$Q$179,3,FALSE)</f>
         <v>75.570454545454538</v>
       </c>
       <c r="M5" s="4">
-        <f>VLOOKUP($J5,$J$44:$Q$179,4,FALSE)</f>
+        <f t="shared" ref="M5:M25" si="2">VLOOKUP($J5,$J$44:$Q$179,4,FALSE)</f>
         <v>75.570454545454538</v>
       </c>
       <c r="N5" s="3">
-        <f>VLOOKUP($J5,$J$44:$Q$179,5,FALSE)</f>
+        <f t="shared" ref="N5:N25" si="3">VLOOKUP($J5,$J$44:$Q$179,5,FALSE)</f>
         <v>1</v>
       </c>
       <c r="P5" s="4">
-        <f>VLOOKUP($J5,$J$44:$Q$179,7,FALSE)</f>
+        <f t="shared" ref="P5:P25" si="4">VLOOKUP($J5,$J$44:$Q$179,7,FALSE)</f>
         <v>4157</v>
       </c>
       <c r="Q5" s="7">
-        <f>VLOOKUP($J5,$J$44:$Q$179,8,FALSE)</f>
+        <f t="shared" ref="Q5:Q25" si="5">VLOOKUP($J5,$J$44:$Q$179,8,FALSE)</f>
         <v>55.008270427957058</v>
       </c>
       <c r="S5" s="1" t="s">
@@ -16607,31 +16607,31 @@
       </c>
       <c r="H6" s="12"/>
       <c r="J6" s="1" t="str">
-        <f t="shared" ref="J6:J23" si="0">A6</f>
+        <f t="shared" ref="J6:J23" si="6">A6</f>
         <v>Sawmill</v>
       </c>
       <c r="K6" s="4">
-        <f>VLOOKUP($J6,$J$44:$Q$179,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>167.22600000000011</v>
       </c>
       <c r="L6" s="4">
-        <f>VLOOKUP($J6,$J$44:$Q$179,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>289.50210000000004</v>
       </c>
       <c r="M6" s="4">
-        <f>VLOOKUP($J6,$J$44:$Q$179,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>16.722600000000011</v>
       </c>
       <c r="N6" s="3">
-        <f>VLOOKUP($J6,$J$44:$Q$179,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>5.7763311561470576E-2</v>
       </c>
       <c r="P6" s="4">
-        <f>VLOOKUP($J6,$J$44:$Q$179,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>21764</v>
       </c>
       <c r="Q6" s="7">
-        <f>VLOOKUP($J6,$J$44:$Q$179,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1301.4722590984647</v>
       </c>
       <c r="S6" s="1" t="s">
@@ -16659,31 +16659,31 @@
       </c>
       <c r="H7" s="12"/>
       <c r="J7" s="1" t="str">
-        <f t="shared" ref="J7" si="1">A7</f>
+        <f t="shared" ref="J7" si="7">A7</f>
         <v>Farm</v>
       </c>
       <c r="K7" s="4">
-        <f>VLOOKUP($J7,$J$44:$Q$179,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>108.486</v>
       </c>
       <c r="L7" s="4">
-        <f>VLOOKUP($J7,$J$44:$Q$179,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>108.486</v>
       </c>
       <c r="M7" s="4">
-        <f>VLOOKUP($J7,$J$44:$Q$179,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>108.486</v>
       </c>
       <c r="N7" s="3">
-        <f>VLOOKUP($J7,$J$44:$Q$179,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="P7" s="4">
-        <f>VLOOKUP($J7,$J$44:$Q$179,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>4157</v>
       </c>
       <c r="Q7" s="7">
-        <f>VLOOKUP($J7,$J$44:$Q$179,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>38.318308353151558</v>
       </c>
       <c r="X7" s="4"/>
@@ -16705,31 +16705,31 @@
       </c>
       <c r="H8" s="12"/>
       <c r="J8" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Iron Mine</v>
+      </c>
+      <c r="K8" s="4">
         <f t="shared" si="0"/>
-        <v>Iron Mine</v>
-      </c>
-      <c r="K8" s="4">
-        <f>VLOOKUP($J8,$J$44:$Q$179,2,FALSE)</f>
         <v>13377.825000000001</v>
       </c>
       <c r="L8" s="4">
-        <f>VLOOKUP($J8,$J$44:$Q$179,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>76.010369318181816</v>
       </c>
       <c r="M8" s="4">
-        <f>VLOOKUP($J8,$J$44:$Q$179,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>76.010369318181816</v>
       </c>
       <c r="N8" s="3">
-        <f>VLOOKUP($J8,$J$44:$Q$179,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="P8" s="4">
-        <f>VLOOKUP($J8,$J$44:$Q$179,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>85018</v>
       </c>
       <c r="Q8" s="7">
-        <f>VLOOKUP($J8,$J$44:$Q$179,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1118.5052876682121</v>
       </c>
       <c r="T8" s="6" t="s">
@@ -16759,31 +16759,31 @@
       </c>
       <c r="H9" s="12"/>
       <c r="J9" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Iron Processing</v>
+      </c>
+      <c r="K9" s="4">
         <f t="shared" si="0"/>
-        <v>Iron Processing</v>
-      </c>
-      <c r="K9" s="4">
-        <f>VLOOKUP($J9,$J$44:$Q$179,2,FALSE)</f>
         <v>2597.9989999999998</v>
       </c>
       <c r="L9" s="4">
-        <f>VLOOKUP($J9,$J$44:$Q$179,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>817.47463636363636</v>
       </c>
       <c r="M9" s="4">
-        <f>VLOOKUP($J9,$J$44:$Q$179,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>236.18172727272724</v>
       </c>
       <c r="N9" s="3">
-        <f>VLOOKUP($J9,$J$44:$Q$179,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.28891627552303262</v>
       </c>
       <c r="P9" s="4">
-        <f>VLOOKUP($J9,$J$44:$Q$179,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>146810</v>
       </c>
       <c r="Q9" s="7">
-        <f>VLOOKUP($J9,$J$44:$Q$179,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>621.59762186205614</v>
       </c>
       <c r="S9" s="1" t="s">
@@ -16818,31 +16818,31 @@
       </c>
       <c r="H10" s="12"/>
       <c r="J10" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Steel Mill</v>
+      </c>
+      <c r="K10" s="4">
         <f t="shared" si="0"/>
-        <v>Steel Mill</v>
-      </c>
-      <c r="K10" s="4">
-        <f>VLOOKUP($J10,$J$44:$Q$179,2,FALSE)</f>
         <v>-37801.909999999996</v>
       </c>
       <c r="L10" s="4">
-        <f>VLOOKUP($J10,$J$44:$Q$179,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>85.814599557522129</v>
       </c>
       <c r="M10" s="4">
-        <f>VLOOKUP($J10,$J$44:$Q$179,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-83.632544247787607</v>
       </c>
       <c r="N10" s="3">
-        <f>VLOOKUP($J10,$J$44:$Q$179,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-0.9745724466351221</v>
       </c>
       <c r="P10" s="4">
-        <f>VLOOKUP($J10,$J$44:$Q$179,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>257030</v>
       </c>
       <c r="Q10" s="7">
-        <f>VLOOKUP($J10,$J$44:$Q$179,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-3073.3251309259244</v>
       </c>
       <c r="S10" s="1" t="s">
@@ -16873,31 +16873,31 @@
       </c>
       <c r="H11" s="12"/>
       <c r="J11" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Coal Mine</v>
+      </c>
+      <c r="K11" s="4">
         <f t="shared" si="0"/>
-        <v>Coal Mine</v>
-      </c>
-      <c r="K11" s="4">
-        <f>VLOOKUP($J11,$J$44:$Q$179,2,FALSE)</f>
         <v>5806.8720000000003</v>
       </c>
       <c r="L11" s="4">
-        <f>VLOOKUP($J11,$J$44:$Q$179,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>30.244125</v>
       </c>
       <c r="M11" s="4">
-        <f>VLOOKUP($J11,$J$44:$Q$179,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>30.244125</v>
       </c>
       <c r="N11" s="3">
-        <f>VLOOKUP($J11,$J$44:$Q$179,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="P11" s="4">
-        <f>VLOOKUP($J11,$J$44:$Q$179,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>84568</v>
       </c>
       <c r="Q11" s="7">
-        <f>VLOOKUP($J11,$J$44:$Q$179,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>2796.1794232764214</v>
       </c>
       <c r="S11" s="1" t="s">
@@ -16929,31 +16929,31 @@
       </c>
       <c r="H12" s="12"/>
       <c r="J12" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Coal Processing</v>
+      </c>
+      <c r="K12" s="4">
         <f t="shared" si="0"/>
-        <v>Coal Processing</v>
-      </c>
-      <c r="K12" s="4">
-        <f>VLOOKUP($J12,$J$44:$Q$179,2,FALSE)</f>
         <v>1719.9180000000006</v>
       </c>
       <c r="L12" s="4">
-        <f>VLOOKUP($J12,$J$44:$Q$179,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>246.62085714285718</v>
       </c>
       <c r="M12" s="4">
-        <f>VLOOKUP($J12,$J$44:$Q$179,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>81.900857142857177</v>
       </c>
       <c r="N12" s="3">
-        <f>VLOOKUP($J12,$J$44:$Q$179,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.33209217619179476</v>
       </c>
       <c r="P12" s="4">
-        <f>VLOOKUP($J12,$J$44:$Q$179,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>146810</v>
       </c>
       <c r="Q12" s="7">
-        <f>VLOOKUP($J12,$J$44:$Q$179,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1792.5331323935204</v>
       </c>
       <c r="S12" s="1" t="s">
@@ -16984,31 +16984,31 @@
       </c>
       <c r="H13" s="12"/>
       <c r="J13" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Brick Factory</v>
+      </c>
+      <c r="K13" s="4">
         <f t="shared" si="0"/>
-        <v>Brick Factory</v>
-      </c>
-      <c r="K13" s="4">
-        <f>VLOOKUP($J13,$J$44:$Q$179,2,FALSE)</f>
         <v>-2049.9059999999999</v>
       </c>
       <c r="L13" s="4">
-        <f>VLOOKUP($J13,$J$44:$Q$179,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>38.247183673469387</v>
       </c>
       <c r="M13" s="4">
-        <f>VLOOKUP($J13,$J$44:$Q$179,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-20.917408163265307</v>
       </c>
       <c r="N13" s="3">
-        <f>VLOOKUP($J13,$J$44:$Q$179,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-0.54690061212990471</v>
       </c>
       <c r="P13" s="4">
-        <f>VLOOKUP($J13,$J$44:$Q$179,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>56668</v>
       </c>
       <c r="Q13" s="7">
-        <f>VLOOKUP($J13,$J$44:$Q$179,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-2709.1310528385206</v>
       </c>
       <c r="S13" s="1" t="s">
@@ -17039,31 +17039,31 @@
       </c>
       <c r="H14" s="12"/>
       <c r="J14" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Coal Power Plant</v>
+      </c>
+      <c r="K14" s="4">
         <f t="shared" si="0"/>
-        <v>Coal Power Plant</v>
-      </c>
-      <c r="K14" s="4">
-        <f>VLOOKUP($J14,$J$44:$Q$179,2,FALSE)</f>
         <v>2335.904</v>
       </c>
       <c r="L14" s="4">
-        <f>VLOOKUP($J14,$J$44:$Q$179,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>160.94808333333333</v>
       </c>
       <c r="M14" s="4">
-        <f>VLOOKUP($J14,$J$44:$Q$179,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>97.329333333333338</v>
       </c>
       <c r="N14" s="3">
-        <f>VLOOKUP($J14,$J$44:$Q$179,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.60472502261339967</v>
       </c>
       <c r="P14" s="4">
-        <f>VLOOKUP($J14,$J$44:$Q$179,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>252962</v>
       </c>
       <c r="Q14" s="7">
-        <f>VLOOKUP($J14,$J$44:$Q$179,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>2599.0314670465909</v>
       </c>
       <c r="S14" s="1" t="s">
@@ -17092,31 +17092,31 @@
       </c>
       <c r="H15" s="12"/>
       <c r="J15" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Quarry</v>
+      </c>
+      <c r="K15" s="4">
         <f t="shared" si="0"/>
-        <v>Quarry</v>
-      </c>
-      <c r="K15" s="4">
-        <f>VLOOKUP($J15,$J$44:$Q$179,2,FALSE)</f>
         <v>947.33979999999997</v>
       </c>
       <c r="L15" s="4">
-        <f>VLOOKUP($J15,$J$44:$Q$179,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>24.290764102564101</v>
       </c>
       <c r="M15" s="4">
-        <f>VLOOKUP($J15,$J$44:$Q$179,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>24.290764102564101</v>
       </c>
       <c r="N15" s="3">
-        <f>VLOOKUP($J15,$J$44:$Q$179,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="P15" s="4">
-        <f>VLOOKUP($J15,$J$44:$Q$179,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>1641</v>
       </c>
       <c r="Q15" s="7">
-        <f>VLOOKUP($J15,$J$44:$Q$179,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>67.556540958165172</v>
       </c>
       <c r="S15" s="1" t="s">
@@ -17147,31 +17147,31 @@
       </c>
       <c r="H16" s="12"/>
       <c r="J16" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Gravel Processing</v>
+      </c>
+      <c r="K16" s="4">
         <f t="shared" si="0"/>
-        <v>Gravel Processing</v>
-      </c>
-      <c r="K16" s="4">
-        <f>VLOOKUP($J16,$J$44:$Q$179,2,FALSE)</f>
         <v>72.184299999999666</v>
       </c>
       <c r="L16" s="4">
-        <f>VLOOKUP($J16,$J$44:$Q$179,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>130.85895333333332</v>
       </c>
       <c r="M16" s="4">
-        <f>VLOOKUP($J16,$J$44:$Q$179,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>4.8122866666666448</v>
       </c>
       <c r="N16" s="3">
-        <f>VLOOKUP($J16,$J$44:$Q$179,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>3.6774607652626128E-2</v>
       </c>
       <c r="P16" s="4">
-        <f>VLOOKUP($J16,$J$44:$Q$179,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>36782</v>
       </c>
       <c r="Q16" s="7">
-        <f>VLOOKUP($J16,$J$44:$Q$179,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>7643.3518091884598</v>
       </c>
       <c r="S16" s="1" t="s">
@@ -17204,31 +17204,31 @@
       </c>
       <c r="H17" s="12"/>
       <c r="J17" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Cement Plant</v>
+      </c>
+      <c r="K17" s="4">
         <f t="shared" si="0"/>
-        <v>Cement Plant</v>
-      </c>
-      <c r="K17" s="4">
-        <f>VLOOKUP($J17,$J$44:$Q$179,2,FALSE)</f>
         <v>-4246.4794999999995</v>
       </c>
       <c r="L17" s="4">
-        <f>VLOOKUP($J17,$J$44:$Q$179,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>188.49914999999999</v>
       </c>
       <c r="M17" s="4">
-        <f>VLOOKUP($J17,$J$44:$Q$179,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-212.32397499999996</v>
       </c>
       <c r="N17" s="3">
-        <f>VLOOKUP($J17,$J$44:$Q$179,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-1.1263922145007019</v>
       </c>
       <c r="P17" s="4">
-        <f>VLOOKUP($J17,$J$44:$Q$179,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>203603</v>
       </c>
       <c r="Q17" s="7">
-        <f>VLOOKUP($J17,$J$44:$Q$179,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-958.92609395618194</v>
       </c>
       <c r="S17" s="1" t="s">
@@ -17261,31 +17261,31 @@
       </c>
       <c r="H18" s="12"/>
       <c r="J18" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Concrete Plant</v>
+      </c>
+      <c r="K18" s="4">
         <f t="shared" si="0"/>
-        <v>Concrete Plant</v>
-      </c>
-      <c r="K18" s="4">
-        <f>VLOOKUP($J18,$J$44:$Q$179,2,FALSE)</f>
         <v>-5816.8510000000006</v>
       </c>
       <c r="L18" s="4">
-        <f>VLOOKUP($J18,$J$44:$Q$179,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>620.13599999999997</v>
       </c>
       <c r="M18" s="4">
-        <f>VLOOKUP($J18,$J$44:$Q$179,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-1454.2127500000001</v>
       </c>
       <c r="N18" s="3">
-        <f>VLOOKUP($J18,$J$44:$Q$179,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-2.3449900505695527</v>
       </c>
       <c r="P18" s="4">
-        <f>VLOOKUP($J18,$J$44:$Q$179,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>34720</v>
       </c>
       <c r="Q18" s="7">
-        <f>VLOOKUP($J18,$J$44:$Q$179,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-23.875461138681391</v>
       </c>
       <c r="S18" s="1" t="s">
@@ -17314,31 +17314,31 @@
       </c>
       <c r="H19" s="12"/>
       <c r="J19" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Oil Rig</v>
+      </c>
+      <c r="K19" s="4">
         <f t="shared" si="0"/>
-        <v>Oil Rig</v>
-      </c>
-      <c r="K19" s="4">
-        <f>VLOOKUP($J19,$J$44:$Q$179,2,FALSE)</f>
         <v>181.79700000000003</v>
       </c>
       <c r="L19" s="4">
-        <f>VLOOKUP($J19,$J$44:$Q$179,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>181.79700000000003</v>
       </c>
       <c r="M19" s="4">
-        <f>VLOOKUP($J19,$J$44:$Q$179,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>181.79700000000003</v>
       </c>
       <c r="N19" s="3">
-        <f>VLOOKUP($J19,$J$44:$Q$179,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="P19" s="4">
-        <f>VLOOKUP($J19,$J$44:$Q$179,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>6069</v>
       </c>
       <c r="Q19" s="7">
-        <f>VLOOKUP($J19,$J$44:$Q$179,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>33.383389164837702</v>
       </c>
       <c r="S19" s="1" t="s">
@@ -17371,31 +17371,31 @@
         <v>49.460999999999999</v>
       </c>
       <c r="J20" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Oil Refinery</v>
+      </c>
+      <c r="K20" s="4">
         <f t="shared" si="0"/>
-        <v>Oil Refinery</v>
-      </c>
-      <c r="K20" s="4">
-        <f>VLOOKUP($J20,$J$44:$Q$179,2,FALSE)</f>
         <v>13374.071999999998</v>
       </c>
       <c r="L20" s="4">
-        <f>VLOOKUP($J20,$J$44:$Q$179,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>66.989904328018227</v>
       </c>
       <c r="M20" s="4">
-        <f>VLOOKUP($J20,$J$44:$Q$179,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>30.46485649202733</v>
       </c>
       <c r="N20" s="3">
-        <f>VLOOKUP($J20,$J$44:$Q$179,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.45476787581088607</v>
       </c>
       <c r="P20" s="4">
-        <f>VLOOKUP($J20,$J$44:$Q$179,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>296868</v>
       </c>
       <c r="Q20" s="7">
-        <f>VLOOKUP($J20,$J$44:$Q$179,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>9744.6052331705723</v>
       </c>
       <c r="S20" s="1" t="s">
@@ -17430,31 +17430,31 @@
       </c>
       <c r="H21" s="12"/>
       <c r="J21" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Asphalt Plant</v>
+      </c>
+      <c r="K21" s="4">
         <f t="shared" si="0"/>
-        <v>Asphalt Plant</v>
-      </c>
-      <c r="K21" s="4">
-        <f>VLOOKUP($J21,$J$44:$Q$179,2,FALSE)</f>
         <v>-11037.831600000001</v>
       </c>
       <c r="L21" s="4">
-        <f>VLOOKUP($J21,$J$44:$Q$179,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1781.82</v>
       </c>
       <c r="M21" s="4">
-        <f>VLOOKUP($J21,$J$44:$Q$179,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-2759.4579000000003</v>
       </c>
       <c r="N21" s="3">
-        <f>VLOOKUP($J21,$J$44:$Q$179,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-1.5486737717614576</v>
       </c>
       <c r="P21" s="4">
-        <f>VLOOKUP($J21,$J$44:$Q$179,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>38940</v>
       </c>
       <c r="Q21" s="7">
-        <f>VLOOKUP($J21,$J$44:$Q$179,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-14.111467328419831</v>
       </c>
       <c r="S21" s="1" t="s">
@@ -17485,31 +17485,31 @@
       </c>
       <c r="H22" s="12"/>
       <c r="J22" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Livestock Farm</v>
+      </c>
+      <c r="K22" s="4">
         <f t="shared" si="0"/>
-        <v>Livestock Farm</v>
-      </c>
-      <c r="K22" s="4">
-        <f>VLOOKUP($J22,$J$44:$Q$179,2,FALSE)</f>
         <v>119.38940000000002</v>
       </c>
       <c r="L22" s="4">
-        <f>VLOOKUP($J22,$J$44:$Q$179,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>23.925428571428572</v>
       </c>
       <c r="M22" s="4">
-        <f>VLOOKUP($J22,$J$44:$Q$179,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>17.055628571428574</v>
       </c>
       <c r="N22" s="3">
-        <f>VLOOKUP($J22,$J$44:$Q$179,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.71286616749662657</v>
       </c>
       <c r="P22" s="4">
-        <f>VLOOKUP($J22,$J$44:$Q$179,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>47934</v>
       </c>
       <c r="Q22" s="7">
-        <f>VLOOKUP($J22,$J$44:$Q$179,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>2810.4505090066614</v>
       </c>
       <c r="S22" s="1" t="s">
@@ -17540,31 +17540,31 @@
       </c>
       <c r="H23" s="12"/>
       <c r="J23" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>Slaughterhouse</v>
+      </c>
+      <c r="K23" s="4">
         <f t="shared" si="0"/>
-        <v>Slaughterhouse</v>
-      </c>
-      <c r="K23" s="4">
-        <f>VLOOKUP($J23,$J$44:$Q$179,2,FALSE)</f>
         <v>-19161.050000000003</v>
       </c>
       <c r="L23" s="4">
-        <f>VLOOKUP($J23,$J$44:$Q$179,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1225.2516666666668</v>
       </c>
       <c r="M23" s="4">
-        <f>VLOOKUP($J23,$J$44:$Q$179,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>-3193.5083333333337</v>
       </c>
       <c r="N23" s="3">
-        <f>VLOOKUP($J23,$J$44:$Q$179,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>-2.6064101116641347</v>
       </c>
       <c r="P23" s="4">
-        <f>VLOOKUP($J23,$J$44:$Q$179,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>35621</v>
       </c>
       <c r="Q23" s="7">
-        <f>VLOOKUP($J23,$J$44:$Q$179,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>-11.154190401882985</v>
       </c>
       <c r="S23" s="1" t="s">
@@ -17595,31 +17595,31 @@
       </c>
       <c r="H24" s="12"/>
       <c r="J24" s="1" t="str">
-        <f t="shared" ref="J24:J33" si="2">A24</f>
+        <f t="shared" ref="J24:J33" si="8">A24</f>
         <v>Food Factory</v>
       </c>
       <c r="K24" s="4">
-        <f>VLOOKUP($J24,$J$44:$Q$179,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>12980.186799999999</v>
       </c>
       <c r="L24" s="4">
-        <f>VLOOKUP($J24,$J$44:$Q$179,3,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>80.21095505617977</v>
       </c>
       <c r="M24" s="4">
-        <f>VLOOKUP($J24,$J$44:$Q$179,4,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>72.92239775280899</v>
       </c>
       <c r="N24" s="3">
-        <f>VLOOKUP($J24,$J$44:$Q$179,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.90913264530679283</v>
       </c>
       <c r="P24" s="4">
-        <f>VLOOKUP($J24,$J$44:$Q$179,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>71504</v>
       </c>
       <c r="Q24" s="7">
-        <f>VLOOKUP($J24,$J$44:$Q$179,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>980.54921674933075</v>
       </c>
       <c r="S24" s="1" t="s">
@@ -17650,31 +17650,31 @@
       </c>
       <c r="H25" s="12"/>
       <c r="J25" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>Distillery</v>
+      </c>
+      <c r="K25" s="4">
+        <f t="shared" si="0"/>
+        <v>3727.038</v>
+      </c>
+      <c r="L25" s="4">
+        <f t="shared" si="1"/>
+        <v>56.938000000000002</v>
+      </c>
+      <c r="M25" s="4">
         <f t="shared" si="2"/>
-        <v>Distillery</v>
-      </c>
-      <c r="K25" s="4">
-        <f>VLOOKUP($J25,$J$44:$Q$179,2,FALSE)</f>
-        <v>3727.038</v>
-      </c>
-      <c r="L25" s="4">
-        <f>VLOOKUP($J25,$J$44:$Q$179,3,FALSE)</f>
-        <v>56.938000000000002</v>
-      </c>
-      <c r="M25" s="4">
-        <f>VLOOKUP($J25,$J$44:$Q$179,4,FALSE)</f>
         <v>46.587975</v>
       </c>
       <c r="N25" s="3">
-        <f>VLOOKUP($J25,$J$44:$Q$179,5,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>0.81822289156626504</v>
       </c>
       <c r="P25" s="4">
-        <f>VLOOKUP($J25,$J$44:$Q$179,7,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>37951</v>
       </c>
       <c r="Q25" s="7">
-        <f>VLOOKUP($J25,$J$44:$Q$179,8,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>814.60934930097312</v>
       </c>
       <c r="S25" s="1" t="s">
@@ -17749,7 +17749,7 @@
       </c>
       <c r="H28" s="12"/>
       <c r="J28" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Fabric Factory</v>
       </c>
       <c r="K28" s="4">
@@ -17846,7 +17846,7 @@
       </c>
       <c r="H31" s="12"/>
       <c r="J31" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Clothing Factory</v>
       </c>
       <c r="K31" s="4">
@@ -17924,7 +17924,7 @@
       </c>
       <c r="H33" s="13"/>
       <c r="J33" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Prefab Factory</v>
       </c>
       <c r="K33" s="4">
@@ -18142,7 +18142,7 @@
         <v>16</v>
       </c>
       <c r="T42" s="4">
-        <f t="shared" ref="T42:T70" si="3">T10-$T$5</f>
+        <f t="shared" ref="T42:T70" si="9">T10-$T$5</f>
         <v>24.7</v>
       </c>
       <c r="U42" s="4">
@@ -18178,7 +18178,7 @@
         <v>17</v>
       </c>
       <c r="T43" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>6.6999999999999993</v>
       </c>
       <c r="U43" s="4">
@@ -18244,11 +18244,11 @@
         <v>18</v>
       </c>
       <c r="T44" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>24.5</v>
       </c>
       <c r="U44" s="4">
-        <f t="shared" ref="U44:U70" si="4">U12+$T$6</f>
+        <f t="shared" ref="U44:U70" si="10">U12+$T$6</f>
         <v>34.299999999999997</v>
       </c>
     </row>
@@ -18257,11 +18257,11 @@
         <v>19</v>
       </c>
       <c r="T45" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2243</v>
       </c>
       <c r="U45" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2486</v>
       </c>
     </row>
@@ -18297,11 +18297,11 @@
         <v>20</v>
       </c>
       <c r="T46" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>57</v>
       </c>
       <c r="U46" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>70</v>
       </c>
     </row>
@@ -18319,11 +18319,11 @@
         <v>21</v>
       </c>
       <c r="T47" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>64</v>
       </c>
       <c r="U47" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>78</v>
       </c>
     </row>
@@ -18355,11 +18355,11 @@
         <v>22</v>
       </c>
       <c r="T48" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>25</v>
       </c>
       <c r="U48" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>35</v>
       </c>
     </row>
@@ -18421,11 +18421,11 @@
         <v>23</v>
       </c>
       <c r="T49" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>77</v>
       </c>
       <c r="U49" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>92</v>
       </c>
     </row>
@@ -18434,11 +18434,11 @@
         <v>24</v>
       </c>
       <c r="T50" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>3414</v>
       </c>
       <c r="U50" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>3781</v>
       </c>
     </row>
@@ -18474,11 +18474,11 @@
         <v>25</v>
       </c>
       <c r="T51" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>111</v>
       </c>
       <c r="U51" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>130</v>
       </c>
     </row>
@@ -18493,11 +18493,11 @@
         <v>26</v>
       </c>
       <c r="T52" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="U52" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>21</v>
       </c>
     </row>
@@ -18529,11 +18529,11 @@
         <v>27</v>
       </c>
       <c r="T53" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>163</v>
       </c>
       <c r="U53" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>187</v>
       </c>
     </row>
@@ -18595,11 +18595,11 @@
         <v>28</v>
       </c>
       <c r="T54" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>27</v>
       </c>
       <c r="U54" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>38</v>
       </c>
     </row>
@@ -18608,11 +18608,11 @@
         <v>29</v>
       </c>
       <c r="T55" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>154</v>
       </c>
       <c r="U55" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>840</v>
       </c>
     </row>
@@ -18648,11 +18648,11 @@
         <v>30</v>
       </c>
       <c r="T56" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>81</v>
       </c>
       <c r="U56" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>97</v>
       </c>
     </row>
@@ -18667,11 +18667,11 @@
         <v>31</v>
       </c>
       <c r="T57" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>434</v>
       </c>
       <c r="U57" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>487</v>
       </c>
     </row>
@@ -18703,11 +18703,11 @@
         <v>32</v>
       </c>
       <c r="T58" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>998</v>
       </c>
       <c r="U58" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>1111</v>
       </c>
     </row>
@@ -18769,11 +18769,11 @@
         <v>33</v>
       </c>
       <c r="T59" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>980</v>
       </c>
       <c r="U59" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>1091</v>
       </c>
     </row>
@@ -18782,11 +18782,11 @@
         <v>34</v>
       </c>
       <c r="T60" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>81</v>
       </c>
       <c r="U60" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>97</v>
       </c>
     </row>
@@ -18822,11 +18822,11 @@
         <v>35</v>
       </c>
       <c r="T61" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>350</v>
       </c>
       <c r="U61" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>394</v>
       </c>
     </row>
@@ -18844,11 +18844,11 @@
         <v>36</v>
       </c>
       <c r="T62" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>13851</v>
       </c>
       <c r="U62" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>15316</v>
       </c>
     </row>
@@ -18880,11 +18880,11 @@
         <v>37</v>
       </c>
       <c r="T63" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>662</v>
       </c>
       <c r="U63" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>779</v>
       </c>
     </row>
@@ -18946,11 +18946,11 @@
         <v>38</v>
       </c>
       <c r="T64" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>618</v>
       </c>
       <c r="U64" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>690</v>
       </c>
     </row>
@@ -18959,11 +18959,11 @@
         <v>39</v>
       </c>
       <c r="T65" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>72</v>
       </c>
       <c r="U65" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>86</v>
       </c>
     </row>
@@ -18999,11 +18999,11 @@
         <v>40</v>
       </c>
       <c r="T66" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>22</v>
       </c>
       <c r="U66" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
     </row>
@@ -19027,11 +19027,11 @@
         <v>41</v>
       </c>
       <c r="T67" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2778</v>
       </c>
       <c r="U67" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>3077</v>
       </c>
     </row>
@@ -19063,11 +19063,11 @@
         <v>42</v>
       </c>
       <c r="T68" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>3427</v>
       </c>
       <c r="U68" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>3795</v>
       </c>
     </row>
@@ -19129,11 +19129,11 @@
         <v>43</v>
       </c>
       <c r="T69" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1321</v>
       </c>
       <c r="U69" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>1467</v>
       </c>
       <c r="V69" s="5"/>
@@ -19143,11 +19143,11 @@
         <v>44</v>
       </c>
       <c r="T70" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>3152</v>
       </c>
       <c r="U70" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>3492</v>
       </c>
       <c r="V70" s="5"/>
@@ -20807,11 +20807,11 @@
         <v>1297.3631999999998</v>
       </c>
       <c r="D139" s="6">
-        <f t="shared" ref="D139" si="5">D138*D136</f>
+        <f t="shared" ref="D139" si="11">D138*D136</f>
         <v>0</v>
       </c>
       <c r="E139" s="6">
-        <f t="shared" ref="E139" si="6">E138*E136</f>
+        <f t="shared" ref="E139" si="12">E138*E136</f>
         <v>0</v>
       </c>
       <c r="F139" s="1"/>

</xml_diff>